<commit_message>
i do not like the track infrastructure column
</commit_message>
<xml_diff>
--- a/TrackModelV2/track.xlsx
+++ b/TrackModelV2/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himes\ECE1140\ECE1140\TrackModelV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC98B15-378B-442E-8582-26AAD1302F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5013EFB-386E-4048-B863-620180E578CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="113">
   <si>
     <t>Block Number</t>
   </si>
@@ -219,13 +219,7 @@
     <t>Release 2.0 of Track data - corrections shown in yellow cells; see red and green line</t>
   </si>
   <si>
-    <t>SWITCH (12-13; 1-13)</t>
-  </si>
-  <si>
     <t>SWITCH FROM YARD (Yard-63)</t>
-  </si>
-  <si>
-    <t>SWITCH (85-86; 100-85)</t>
   </si>
   <si>
     <t>STATION; PENN STATION; UNDERGROUND</t>
@@ -241,9 +235,6 @@
   </si>
   <si>
     <t>SWITCH (52-53; 52-66)</t>
-  </si>
-  <si>
-    <t>SWITCH (29-30; 29-150)</t>
   </si>
   <si>
     <t>seconds to traverse block</t>
@@ -348,9 +339,6 @@
     <t>12,9</t>
   </si>
   <si>
-    <t>STATION; MT LEBANON; SWITCH (76-77;77-101)</t>
-  </si>
-  <si>
     <t>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-yard)</t>
   </si>
   <si>
@@ -367,6 +355,24 @@
   </si>
   <si>
     <t>STATION;</t>
+  </si>
+  <si>
+    <t>SWITCH; (12-13; 1-13)</t>
+  </si>
+  <si>
+    <t>SWITCH; (29-30; 29-150)</t>
+  </si>
+  <si>
+    <t>STATION; MT LEBANON; SWITCH; (76-77;77-101)</t>
+  </si>
+  <si>
+    <t>SWITCH; (85-86; 100-85)</t>
+  </si>
+  <si>
+    <t>STATION; OVERBROOK; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>Transition Override</t>
   </si>
 </sst>
 </file>
@@ -1752,7 +1758,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1894,7 +1900,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="12">
@@ -1927,7 +1933,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="12">
@@ -2053,7 +2059,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="12">
@@ -2086,7 +2092,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="12">
@@ -2212,7 +2218,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="12">
@@ -2246,7 +2252,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2259,9 +2265,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2274,7 +2280,9 @@
     <col min="6" max="6" width="13.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="43" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" customWidth="1"/>
-    <col min="9" max="12" width="8.85546875" style="1"/>
+    <col min="9" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1"/>
     <col min="13" max="13" width="11.42578125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -2302,7 +2310,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>35</v>
@@ -2310,9 +2318,11 @@
       <c r="J1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="7"/>
+      <c r="K1" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="L1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2344,7 +2354,7 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2532,7 +2542,7 @@
         <v>37</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
@@ -2599,7 +2609,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
@@ -2610,7 +2620,7 @@
         <v>4.125</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2826,10 +2836,10 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
@@ -2996,7 +3006,7 @@
         <v>58</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
@@ -3130,10 +3140,10 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -3200,7 +3210,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -3339,7 +3349,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3371,7 +3381,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3392,7 +3402,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I34" s="12">
         <f t="shared" si="0"/>
@@ -3402,8 +3412,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3435,7 +3448,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3459,7 +3472,7 @@
         <v>38</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I36" s="12">
         <f t="shared" si="0"/>
@@ -3470,7 +3483,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3502,7 +3515,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -3534,7 +3547,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3555,7 +3568,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -3566,7 +3579,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3598,7 +3611,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3630,7 +3643,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3662,7 +3675,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3694,7 +3707,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3726,7 +3739,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3747,7 +3760,7 @@
         <v>70</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I45" s="12">
         <f t="shared" si="0"/>
@@ -3757,8 +3770,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3779,10 +3795,10 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="0"/>
@@ -3793,7 +3809,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3825,7 +3841,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3881,7 +3897,7 @@
         <v>39</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I49" s="12">
         <f t="shared" si="0"/>
@@ -4000,7 +4016,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -4238,7 +4254,7 @@
         <v>40</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I61" s="12">
         <f t="shared" si="0"/>
@@ -5291,9 +5307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5334,7 +5350,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>35</v>
@@ -5343,13 +5359,13 @@
         <v>36</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -5384,10 +5400,10 @@
         <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -5414,7 +5430,7 @@
         <v>48</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="1">E3*D3/100</f>
@@ -5432,7 +5448,7 @@
         <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5472,7 +5488,7 @@
         <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -5511,7 +5527,7 @@
         <v>14</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -5550,7 +5566,7 @@
         <v>14</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -5589,7 +5605,7 @@
         <v>14</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5629,7 +5645,7 @@
         <v>14</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5668,7 +5684,7 @@
         <v>14</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -5695,7 +5711,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
@@ -5713,7 +5729,7 @@
         <v>14</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5752,7 +5768,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -5791,7 +5807,7 @@
         <v>14</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -5827,10 +5843,10 @@
         <v>8</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -5854,7 +5870,7 @@
         <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
@@ -5869,10 +5885,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5908,10 +5924,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -5947,10 +5963,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -5974,10 +5990,10 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
@@ -5992,10 +6008,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -6031,10 +6047,10 @@
         <v>9</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -6070,10 +6086,10 @@
         <v>9</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -6112,10 +6128,10 @@
         <v>9</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6151,10 +6167,10 @@
         <v>9</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6190,10 +6206,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -6220,7 +6236,7 @@
         <v>50</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="1"/>
@@ -6235,10 +6251,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -6274,10 +6290,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -6313,10 +6329,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -6352,10 +6368,10 @@
         <v>10.285714285714286</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6391,10 +6407,10 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -6430,10 +6446,10 @@
         <v>6</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -6469,10 +6485,10 @@
         <v>6</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -6496,7 +6512,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="1"/>
@@ -6511,10 +6527,10 @@
         <v>6</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -6550,10 +6566,10 @@
         <v>6</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -6580,7 +6596,7 @@
         <v>51</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="1"/>
@@ -6598,7 +6614,7 @@
         <v>11</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -6637,7 +6653,7 @@
         <v>11</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -6676,7 +6692,7 @@
         <v>11</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -6715,7 +6731,7 @@
         <v>11</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -6754,7 +6770,7 @@
         <v>11</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -6793,10 +6809,10 @@
         <v>6</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -6838,7 +6854,7 @@
         <v>10</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -6880,7 +6896,7 @@
         <v>10</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -6907,7 +6923,7 @@
         <v>56</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="1"/>
@@ -6925,7 +6941,7 @@
         <v>10</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -6967,7 +6983,7 @@
         <v>10</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -7009,7 +7025,7 @@
         <v>10</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7051,7 +7067,7 @@
         <v>10</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7093,7 +7109,7 @@
         <v>10</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7135,7 +7151,7 @@
         <v>10</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7177,7 +7193,7 @@
         <v>10</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -7219,7 +7235,7 @@
         <v>10</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -7261,7 +7277,7 @@
         <v>10</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -7288,7 +7304,7 @@
         <v>57</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="1"/>
@@ -7306,7 +7322,7 @@
         <v>10</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -7348,7 +7364,7 @@
         <v>10</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -7390,7 +7406,7 @@
         <v>10</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -7432,7 +7448,7 @@
         <v>10</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -7474,7 +7490,7 @@
         <v>10</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7516,7 +7532,7 @@
         <v>10</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -7558,7 +7574,7 @@
         <v>10</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -7600,7 +7616,7 @@
         <v>10</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7642,7 +7658,7 @@
         <v>10</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
@@ -7666,10 +7682,10 @@
         <v>30</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="1"/>
@@ -7687,7 +7703,7 @@
         <v>10</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -7724,10 +7740,10 @@
         <v>6</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -7766,7 +7782,7 @@
         <v>0</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -7805,7 +7821,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -7844,7 +7860,7 @@
         <v>0</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -7881,10 +7897,10 @@
         <v>6</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -7908,7 +7924,7 @@
         <v>70</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I64" s="3">
         <f t="shared" si="1"/>
@@ -7926,7 +7942,7 @@
         <v>1</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -7965,7 +7981,7 @@
         <v>1</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -7992,7 +8008,7 @@
         <v>52</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="1"/>
@@ -8010,7 +8026,7 @@
         <v>1</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -8049,7 +8065,7 @@
         <v>1</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -8088,7 +8104,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -8124,10 +8140,10 @@
         <v>9</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -8166,7 +8182,7 @@
         <v>2</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -8205,7 +8221,7 @@
         <v>2</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -8244,7 +8260,7 @@
         <v>2</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -8283,7 +8299,7 @@
         <v>2</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -8310,7 +8326,7 @@
         <v>53</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="5"/>
@@ -8328,7 +8344,7 @@
         <v>2</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -8367,7 +8383,7 @@
         <v>2</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -8406,7 +8422,7 @@
         <v>2</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -8442,10 +8458,10 @@
         <v>9</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -8469,10 +8485,10 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="8">E78*D78/100</f>
@@ -8487,10 +8503,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -8526,10 +8542,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -8565,10 +8581,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -8604,10 +8620,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -8643,10 +8659,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -8682,10 +8698,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -8721,10 +8737,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -8760,10 +8776,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -8787,7 +8803,7 @@
         <v>70</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="I86" s="3">
         <f t="shared" si="8"/>
@@ -8802,10 +8818,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -8841,10 +8857,10 @@
         <v>14.399999999999999</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -8883,7 +8899,7 @@
         <v>5</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -8910,7 +8926,7 @@
         <v>54</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="8"/>
@@ -8928,7 +8944,7 @@
         <v>5</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -8967,7 +8983,7 @@
         <v>5</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -9006,7 +9022,7 @@
         <v>5</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -9045,7 +9061,7 @@
         <v>5</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -9084,7 +9100,7 @@
         <v>5</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -9123,7 +9139,7 @@
         <v>5</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -9162,7 +9178,7 @@
         <v>5</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -9201,7 +9217,7 @@
         <v>5</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -9228,7 +9244,7 @@
         <v>55</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="8"/>
@@ -9246,7 +9262,7 @@
         <v>5</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -9285,7 +9301,7 @@
         <v>5</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -9324,7 +9340,7 @@
         <v>5</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -9363,7 +9379,7 @@
         <v>5</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -9399,10 +9415,10 @@
         <v>10.799999999999999</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -9438,10 +9454,10 @@
         <v>4.8461538461538467</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -9480,7 +9496,7 @@
         <v>6</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -9519,7 +9535,7 @@
         <v>6</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -9558,7 +9574,7 @@
         <v>6</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -9586,7 +9602,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I106" s="3">
         <f t="shared" si="8"/>
@@ -9604,7 +9620,7 @@
         <v>6</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -9643,7 +9659,7 @@
         <v>6</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -9682,7 +9698,7 @@
         <v>6</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -9721,7 +9737,7 @@
         <v>6</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -9760,7 +9776,7 @@
         <v>6</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -9796,10 +9812,10 @@
         <v>12</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -9838,7 +9854,7 @@
         <v>7</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -9877,7 +9893,7 @@
         <v>7</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -9916,7 +9932,7 @@
         <v>7</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -9945,7 +9961,7 @@
         <v>STATION; GLENBURY</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I115" s="3">
         <f t="shared" si="10"/>
@@ -9963,7 +9979,7 @@
         <v>7</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -10002,7 +10018,7 @@
         <v>7</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -10041,7 +10057,7 @@
         <v>7</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -10080,7 +10096,7 @@
         <v>7</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
@@ -10119,7 +10135,7 @@
         <v>7</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -10158,7 +10174,7 @@
         <v>7</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -10197,7 +10213,7 @@
         <v>7</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -10236,7 +10252,7 @@
         <v>7</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -10275,13 +10291,13 @@
         <v>9</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="124" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -10301,12 +10317,11 @@
       <c r="F124" s="3">
         <v>20</v>
       </c>
-      <c r="G124" s="11" t="str">
-        <f>G58</f>
-        <v>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-yard)</v>
+      <c r="G124" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I124" s="3">
         <f t="shared" si="10"/>
@@ -10324,7 +10339,7 @@
         <v>8</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -10366,7 +10381,7 @@
         <v>8</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -10408,7 +10423,7 @@
         <v>8</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -10450,7 +10465,7 @@
         <v>8</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -10492,7 +10507,7 @@
         <v>8</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -10534,7 +10549,7 @@
         <v>8</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
@@ -10576,7 +10591,7 @@
         <v>8</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -10618,7 +10633,7 @@
         <v>8</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -10660,7 +10675,7 @@
         <v>8</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -10688,7 +10703,7 @@
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I133" s="3">
         <f t="shared" si="10"/>
@@ -10706,7 +10721,7 @@
         <v>8</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
@@ -10748,7 +10763,7 @@
         <v>8</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -10790,7 +10805,7 @@
         <v>8</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -10832,7 +10847,7 @@
         <v>8</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -10874,7 +10889,7 @@
         <v>8</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -10916,7 +10931,7 @@
         <v>8</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -10958,7 +10973,7 @@
         <v>8</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -11000,7 +11015,7 @@
         <v>8</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -11042,7 +11057,7 @@
         <v>8</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -11070,7 +11085,7 @@
         <v>STATION; CENTRAL; UNDERDROUND</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I142" s="3">
         <f t="shared" si="10"/>
@@ -11088,7 +11103,7 @@
         <v>8</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
@@ -11130,7 +11145,7 @@
         <v>8</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -11172,7 +11187,7 @@
         <v>8</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -11208,10 +11223,10 @@
         <v>9</v>
       </c>
       <c r="M145" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -11250,7 +11265,7 @@
         <v>9</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -11289,7 +11304,7 @@
         <v>9</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -11328,7 +11343,7 @@
         <v>9</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -11368,7 +11383,7 @@
         <v>9</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -11407,7 +11422,7 @@
         <v>9</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -11443,10 +11458,10 @@
         <v>6.3</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -11535,7 +11550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="C7" zoomScale="87" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
excel parser finished but will explode if used
</commit_message>
<xml_diff>
--- a/TrackModelV2/track.xlsx
+++ b/TrackModelV2/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himes\ECE1140\ECE1140\TrackModelV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5013EFB-386E-4048-B863-620180E578CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65D5E69-4E40-4FE1-84A0-39D11717FD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="975" windowWidth="27780" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>Release 2.0 of Track data - corrections shown in yellow cells; see red and green line</t>
   </si>
   <si>
-    <t>SWITCH FROM YARD (Yard-63)</t>
-  </si>
-  <si>
     <t>STATION; PENN STATION; UNDERGROUND</t>
   </si>
   <si>
@@ -339,18 +336,6 @@
     <t>12,9</t>
   </si>
   <si>
-    <t>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-yard)</t>
-  </si>
-  <si>
-    <t>UNDERGROUND; SWITCH (43-44; 44-67)</t>
-  </si>
-  <si>
-    <t>UNDERGROUND; SWITCH (32-33; 33-72)</t>
-  </si>
-  <si>
-    <t>STATION: HERRON AVE; SWITCH (15-16; 1-16)</t>
-  </si>
-  <si>
     <t>SWITCH TO/FROM YARD (10-yard)</t>
   </si>
   <si>
@@ -363,16 +348,31 @@
     <t>SWITCH; (29-30; 29-150)</t>
   </si>
   <si>
-    <t>STATION; MT LEBANON; SWITCH; (76-77;77-101)</t>
-  </si>
-  <si>
-    <t>SWITCH; (85-86; 100-85)</t>
-  </si>
-  <si>
     <t>STATION; OVERBROOK; UNDERGROUND</t>
   </si>
   <si>
     <t>Transition Override</t>
+  </si>
+  <si>
+    <t>SWITCH FROM YARD; (Yard-63)</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; SWITCH TO YARD; (57-yard); STATION; OVERBROOK</t>
+  </si>
+  <si>
+    <t>SWITCH; (76-77;101-77); STATION; MT LEBANON</t>
+  </si>
+  <si>
+    <t>SWITCH; (85-86; 85-100)</t>
+  </si>
+  <si>
+    <t>SWITCH (15-16; 1-16); STATION: HERRON AVE</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; SWITCH (32-33; 72-33)</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; SWITCH (43-44; 67-44)</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1900,7 +1900,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="12">
@@ -1933,7 +1933,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="12">
@@ -2059,7 +2059,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="12">
@@ -2092,7 +2092,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="12">
@@ -2218,7 +2218,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="12">
@@ -2252,7 +2252,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2266,8 +2266,8 @@
   <dimension ref="A1:L154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2310,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>35</v>
@@ -2319,10 +2319,10 @@
         <v>36</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2542,7 +2542,7 @@
         <v>37</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
@@ -2608,9 +2608,7 @@
       <c r="F10" s="3">
         <v>40</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="G10" s="11"/>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2620,7 +2618,7 @@
         <v>4.125</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2643,6 +2641,9 @@
       <c r="F11" s="3">
         <v>40</v>
       </c>
+      <c r="G11" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="I11" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2836,10 +2837,10 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
@@ -3006,7 +3007,7 @@
         <v>58</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
@@ -3140,10 +3141,10 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -3210,7 +3211,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -3402,7 +3403,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="I34" s="12">
         <f t="shared" si="0"/>
@@ -3472,7 +3473,7 @@
         <v>38</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I36" s="12">
         <f t="shared" si="0"/>
@@ -3568,7 +3569,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -3760,7 +3761,7 @@
         <v>70</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="I45" s="12">
         <f t="shared" si="0"/>
@@ -3795,10 +3796,10 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="0"/>
@@ -3897,7 +3898,7 @@
         <v>39</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I49" s="12">
         <f t="shared" si="0"/>
@@ -4016,7 +4017,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -4254,7 +4255,7 @@
         <v>40</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I61" s="12">
         <f t="shared" si="0"/>
@@ -5308,8 +5309,8 @@
   <dimension ref="A1:N151"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5350,7 +5351,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>35</v>
@@ -5359,13 +5360,13 @@
         <v>36</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -5400,10 +5401,10 @@
         <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -5430,7 +5431,7 @@
         <v>48</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="1">E3*D3/100</f>
@@ -5448,7 +5449,7 @@
         <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5488,7 +5489,7 @@
         <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -5527,7 +5528,7 @@
         <v>14</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -5566,7 +5567,7 @@
         <v>14</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -5605,7 +5606,7 @@
         <v>14</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5645,7 +5646,7 @@
         <v>14</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5684,7 +5685,7 @@
         <v>14</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -5711,7 +5712,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
@@ -5729,7 +5730,7 @@
         <v>14</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5768,7 +5769,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -5807,7 +5808,7 @@
         <v>14</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -5843,10 +5844,10 @@
         <v>8</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -5870,7 +5871,7 @@
         <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
@@ -5885,10 +5886,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5924,10 +5925,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -5963,10 +5964,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -5990,10 +5991,10 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
@@ -6008,10 +6009,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -6047,10 +6048,10 @@
         <v>9</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -6086,10 +6087,10 @@
         <v>9</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -6128,10 +6129,10 @@
         <v>9</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6167,10 +6168,10 @@
         <v>9</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6206,10 +6207,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -6236,7 +6237,7 @@
         <v>50</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="1"/>
@@ -6251,10 +6252,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -6290,10 +6291,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -6329,10 +6330,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -6368,10 +6369,10 @@
         <v>10.285714285714286</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6407,10 +6408,10 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -6446,10 +6447,10 @@
         <v>6</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -6485,10 +6486,10 @@
         <v>6</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -6512,7 +6513,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="1"/>
@@ -6527,10 +6528,10 @@
         <v>6</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -6566,10 +6567,10 @@
         <v>6</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -6596,7 +6597,7 @@
         <v>51</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="1"/>
@@ -6614,7 +6615,7 @@
         <v>11</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -6653,7 +6654,7 @@
         <v>11</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -6692,7 +6693,7 @@
         <v>11</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -6731,7 +6732,7 @@
         <v>11</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -6770,7 +6771,7 @@
         <v>11</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -6809,10 +6810,10 @@
         <v>6</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -6854,7 +6855,7 @@
         <v>10</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -6896,7 +6897,7 @@
         <v>10</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -6923,7 +6924,7 @@
         <v>56</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="1"/>
@@ -6941,7 +6942,7 @@
         <v>10</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -6983,7 +6984,7 @@
         <v>10</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -7025,7 +7026,7 @@
         <v>10</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7067,7 +7068,7 @@
         <v>10</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7109,7 +7110,7 @@
         <v>10</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7151,7 +7152,7 @@
         <v>10</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7193,7 +7194,7 @@
         <v>10</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -7235,7 +7236,7 @@
         <v>10</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -7277,7 +7278,7 @@
         <v>10</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -7304,7 +7305,7 @@
         <v>57</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="1"/>
@@ -7322,7 +7323,7 @@
         <v>10</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -7364,7 +7365,7 @@
         <v>10</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -7406,7 +7407,7 @@
         <v>10</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -7448,7 +7449,7 @@
         <v>10</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -7490,7 +7491,7 @@
         <v>10</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7532,7 +7533,7 @@
         <v>10</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -7574,7 +7575,7 @@
         <v>10</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -7616,7 +7617,7 @@
         <v>10</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7658,7 +7659,7 @@
         <v>10</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
@@ -7682,10 +7683,10 @@
         <v>30</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="1"/>
@@ -7703,7 +7704,7 @@
         <v>10</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -7740,10 +7741,10 @@
         <v>6</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -7782,7 +7783,7 @@
         <v>0</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -7821,7 +7822,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -7860,7 +7861,7 @@
         <v>0</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -7897,10 +7898,10 @@
         <v>6</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -7924,7 +7925,7 @@
         <v>70</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="I64" s="3">
         <f t="shared" si="1"/>
@@ -7942,7 +7943,7 @@
         <v>1</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -7981,7 +7982,7 @@
         <v>1</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -8008,7 +8009,7 @@
         <v>52</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="1"/>
@@ -8026,7 +8027,7 @@
         <v>1</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -8065,7 +8066,7 @@
         <v>1</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -8104,7 +8105,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -8140,10 +8141,10 @@
         <v>9</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -8182,7 +8183,7 @@
         <v>2</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -8221,7 +8222,7 @@
         <v>2</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -8260,7 +8261,7 @@
         <v>2</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -8299,7 +8300,7 @@
         <v>2</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -8326,7 +8327,7 @@
         <v>53</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="5"/>
@@ -8344,7 +8345,7 @@
         <v>2</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -8383,7 +8384,7 @@
         <v>2</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -8422,7 +8423,7 @@
         <v>2</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -8458,10 +8459,10 @@
         <v>9</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -8485,10 +8486,10 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="8">E78*D78/100</f>
@@ -8503,10 +8504,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -8542,10 +8543,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -8581,10 +8582,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -8620,10 +8621,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -8659,10 +8660,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -8698,10 +8699,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -8737,10 +8738,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -8776,10 +8777,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -8803,7 +8804,7 @@
         <v>70</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I86" s="3">
         <f t="shared" si="8"/>
@@ -8818,10 +8819,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -8857,10 +8858,10 @@
         <v>14.399999999999999</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -8899,7 +8900,7 @@
         <v>5</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -8926,7 +8927,7 @@
         <v>54</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="8"/>
@@ -8944,7 +8945,7 @@
         <v>5</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -8983,7 +8984,7 @@
         <v>5</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -9022,7 +9023,7 @@
         <v>5</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -9061,7 +9062,7 @@
         <v>5</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -9100,7 +9101,7 @@
         <v>5</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -9139,7 +9140,7 @@
         <v>5</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -9178,7 +9179,7 @@
         <v>5</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -9217,7 +9218,7 @@
         <v>5</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -9244,7 +9245,7 @@
         <v>55</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="8"/>
@@ -9262,7 +9263,7 @@
         <v>5</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -9301,7 +9302,7 @@
         <v>5</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -9340,7 +9341,7 @@
         <v>5</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -9379,7 +9380,7 @@
         <v>5</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -9415,10 +9416,10 @@
         <v>10.799999999999999</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -9454,10 +9455,10 @@
         <v>4.8461538461538467</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -9496,7 +9497,7 @@
         <v>6</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -9535,7 +9536,7 @@
         <v>6</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -9574,7 +9575,7 @@
         <v>6</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -9602,7 +9603,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I106" s="3">
         <f t="shared" si="8"/>
@@ -9620,7 +9621,7 @@
         <v>6</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -9659,7 +9660,7 @@
         <v>6</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -9698,7 +9699,7 @@
         <v>6</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -9737,7 +9738,7 @@
         <v>6</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -9776,7 +9777,7 @@
         <v>6</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -9812,10 +9813,10 @@
         <v>12</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -9854,7 +9855,7 @@
         <v>7</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -9893,7 +9894,7 @@
         <v>7</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -9932,7 +9933,7 @@
         <v>7</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -9961,7 +9962,7 @@
         <v>STATION; GLENBURY</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I115" s="3">
         <f t="shared" si="10"/>
@@ -9979,7 +9980,7 @@
         <v>7</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -10018,7 +10019,7 @@
         <v>7</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -10057,7 +10058,7 @@
         <v>7</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -10096,7 +10097,7 @@
         <v>7</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
@@ -10135,7 +10136,7 @@
         <v>7</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -10174,7 +10175,7 @@
         <v>7</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -10213,7 +10214,7 @@
         <v>7</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -10252,7 +10253,7 @@
         <v>7</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -10291,10 +10292,10 @@
         <v>9</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -10318,10 +10319,10 @@
         <v>20</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I124" s="3">
         <f t="shared" si="10"/>
@@ -10339,7 +10340,7 @@
         <v>8</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -10381,7 +10382,7 @@
         <v>8</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -10423,7 +10424,7 @@
         <v>8</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -10465,7 +10466,7 @@
         <v>8</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -10507,7 +10508,7 @@
         <v>8</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -10549,7 +10550,7 @@
         <v>8</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
@@ -10591,7 +10592,7 @@
         <v>8</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -10633,7 +10634,7 @@
         <v>8</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -10675,7 +10676,7 @@
         <v>8</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -10703,7 +10704,7 @@
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I133" s="3">
         <f t="shared" si="10"/>
@@ -10721,7 +10722,7 @@
         <v>8</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
@@ -10763,7 +10764,7 @@
         <v>8</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -10805,7 +10806,7 @@
         <v>8</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -10847,7 +10848,7 @@
         <v>8</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -10889,7 +10890,7 @@
         <v>8</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -10931,7 +10932,7 @@
         <v>8</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -10973,7 +10974,7 @@
         <v>8</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -11015,7 +11016,7 @@
         <v>8</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -11057,7 +11058,7 @@
         <v>8</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -11085,7 +11086,7 @@
         <v>STATION; CENTRAL; UNDERDROUND</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I142" s="3">
         <f t="shared" si="10"/>
@@ -11103,7 +11104,7 @@
         <v>8</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
@@ -11145,7 +11146,7 @@
         <v>8</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -11187,7 +11188,7 @@
         <v>8</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -11223,10 +11224,10 @@
         <v>9</v>
       </c>
       <c r="M145" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -11265,7 +11266,7 @@
         <v>9</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -11304,7 +11305,7 @@
         <v>9</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -11343,7 +11344,7 @@
         <v>9</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -11383,7 +11384,7 @@
         <v>9</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -11422,7 +11423,7 @@
         <v>9</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -11458,10 +11459,10 @@
         <v>6.3</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -11473,7 +11474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
track model opens in main but gui is scuffed
</commit_message>
<xml_diff>
--- a/TrackModelV2/track.xlsx
+++ b/TrackModelV2/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himes\ECE1140\ECE1140\TrackModelV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65D5E69-4E40-4FE1-84A0-39D11717FD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8980DB8-A3D5-48F5-AED5-A4F1FB2A1726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="975" windowWidth="27780" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="105" windowWidth="27780" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="108">
   <si>
     <t>Block Number</t>
   </si>
@@ -138,16 +138,10 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>ELEVATION (M)</t>
   </si>
   <si>
     <t>CUMALTIVE ELEVATION (M)</t>
-  </si>
-  <si>
-    <t>STATION: SHADYSIDE</t>
   </si>
   <si>
     <t>STATION;     STEEL PLAZA; UNDERGROUND</t>
@@ -222,16 +216,7 @@
     <t>STATION; PENN STATION; UNDERGROUND</t>
   </si>
   <si>
-    <t>SWITCH (27-28; 27-76); UNDERGROUND</t>
-  </si>
-  <si>
-    <t>SWITCH (38-39; 38-71); UNDERGROUND</t>
-  </si>
-  <si>
     <t>STATION; FIRST AVE; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>SWITCH (52-53; 52-66)</t>
   </si>
   <si>
     <t>seconds to traverse block</t>
@@ -240,22 +225,10 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>Switch ( 5 to 6)</t>
-  </si>
-  <si>
-    <t>Switch ( 5 to 6) or (5 to 11)</t>
-  </si>
-  <si>
-    <t>Switch (5 to 11)</t>
-  </si>
-  <si>
     <t>Station C</t>
   </si>
   <si>
     <t>Station B</t>
-  </si>
-  <si>
-    <t>Yard</t>
   </si>
   <si>
     <t>Station Side</t>
@@ -336,9 +309,6 @@
     <t>12,9</t>
   </si>
   <si>
-    <t>SWITCH TO/FROM YARD (10-yard)</t>
-  </si>
-  <si>
     <t>STATION;</t>
   </si>
   <si>
@@ -366,13 +336,28 @@
     <t>SWITCH; (85-86; 85-100)</t>
   </si>
   <si>
-    <t>SWITCH (15-16; 1-16); STATION: HERRON AVE</t>
+    <t>SWITCH ;(15-16; 1-16); STATION: HERRON AVE</t>
   </si>
   <si>
-    <t>UNDERGROUND; SWITCH (32-33; 72-33)</t>
+    <t>SWITCH TO/FROM YARD ;(10-yard)</t>
   </si>
   <si>
-    <t>UNDERGROUND; SWITCH (43-44; 67-44)</t>
+    <t>SWITCH; (27-28; 27-76); UNDERGROUND</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; SWITCH ;(32-33; 72-33)</t>
+  </si>
+  <si>
+    <t>SWITCH; (38-39; 38-71); UNDERGROUND</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; SWITCH ;(43-44; 67-44)</t>
+  </si>
+  <si>
+    <t>SWITCH ;(52-53; 52-66)</t>
+  </si>
+  <si>
+    <t>STATION; SHADYSIDE</t>
   </si>
 </sst>
 </file>
@@ -540,405 +525,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3066609" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="TextBox 43">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0518D34-902E-4EBF-9A22-1DBABAC59FB4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="991962">
-          <a:off x="3924720" y="5676900"/>
-          <a:ext cx="3066609" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>11                12                 13               14                    15</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>37440</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>148990</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>216730</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>169310</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="47" name="Group 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD9B0EC4-FB0F-4329-BDC6-0B3DB93B4A1A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="37440" y="4130440"/>
-          <a:ext cx="6818215" cy="2687320"/>
-          <a:chOff x="37440" y="4060590"/>
-          <a:chExt cx="6967440" cy="2598420"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-        <mc:Choice Requires="xdr14">
-          <xdr14:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-            <xdr14:nvContentPartPr>
-              <xdr14:cNvPr id="32" name="Ink 31">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D70448D-3CF3-459D-BFB7-8B7398F9DF72}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr14:cNvPr>
-              <xdr14:cNvContentPartPr/>
-            </xdr14:nvContentPartPr>
-            <xdr14:nvPr macro=""/>
-            <xdr14:xfrm>
-              <a:off x="723600" y="4060590"/>
-              <a:ext cx="5337360" cy="1179720"/>
-            </xdr14:xfrm>
-          </xdr14:contentPart>
-        </mc:Choice>
-        <mc:Fallback xmlns="">
-          <xdr:pic>
-            <xdr:nvPicPr>
-              <xdr:cNvPr id="32" name="Ink 31">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D70448D-3CF3-459D-BFB7-8B7398F9DF72}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvPicPr/>
-            </xdr:nvPicPr>
-            <xdr:blipFill>
-              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-              <a:stretch>
-                <a:fillRect/>
-              </a:stretch>
-            </xdr:blipFill>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="705600" y="4042950"/>
-                <a:ext cx="5373000" cy="1215360"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-          </xdr:pic>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-        <mc:Choice Requires="xdr14">
-          <xdr14:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
-            <xdr14:nvContentPartPr>
-              <xdr14:cNvPr id="41" name="Ink 40">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB5EE961-6407-4AA5-B8C2-8BFB44A9EA37}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr14:cNvPr>
-              <xdr14:cNvContentPartPr/>
-            </xdr14:nvContentPartPr>
-            <xdr14:nvPr macro=""/>
-            <xdr14:xfrm>
-              <a:off x="3740040" y="5308360"/>
-              <a:ext cx="3264840" cy="1155240"/>
-            </xdr14:xfrm>
-          </xdr14:contentPart>
-        </mc:Choice>
-        <mc:Fallback xmlns="">
-          <xdr:pic>
-            <xdr:nvPicPr>
-              <xdr:cNvPr id="41" name="Ink 40">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB5EE961-6407-4AA5-B8C2-8BFB44A9EA37}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvPicPr/>
-            </xdr:nvPicPr>
-            <xdr:blipFill>
-              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-              <a:stretch>
-                <a:fillRect/>
-              </a:stretch>
-            </xdr:blipFill>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="3722040" y="5290715"/>
-                <a:ext cx="3300480" cy="1190891"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-          </xdr:pic>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-        <mc:Choice Requires="xdr14">
-          <xdr14:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
-            <xdr14:nvContentPartPr>
-              <xdr14:cNvPr id="42" name="Ink 41">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397CF852-D100-4BC1-B0A3-512C2172730C}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr14:cNvPr>
-              <xdr14:cNvContentPartPr/>
-            </xdr14:nvContentPartPr>
-            <xdr14:nvPr macro=""/>
-            <xdr14:xfrm>
-              <a:off x="37440" y="4831870"/>
-              <a:ext cx="559800" cy="1037160"/>
-            </xdr14:xfrm>
-          </xdr14:contentPart>
-        </mc:Choice>
-        <mc:Fallback xmlns="">
-          <xdr:pic>
-            <xdr:nvPicPr>
-              <xdr:cNvPr id="42" name="Ink 41">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397CF852-D100-4BC1-B0A3-512C2172730C}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvPicPr/>
-            </xdr:nvPicPr>
-            <xdr:blipFill>
-              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-              <a:stretch>
-                <a:fillRect/>
-              </a:stretch>
-            </xdr:blipFill>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="19440" y="4813870"/>
-                <a:ext cx="595440" cy="1072800"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-          </xdr:pic>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="43" name="TextBox 42">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7553888-AF3F-4C2E-8490-91185DA1BB90}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="19988673">
-            <a:off x="3722226" y="4343399"/>
-            <a:ext cx="2334485" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>6            7              8               9             10</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="45" name="TextBox 44">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5815E7FD-B5AC-4770-AEDE-E8EB49B3C9AD}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="19627616">
-            <a:off x="5588000" y="4191000"/>
-            <a:ext cx="701089" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Station B</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="46" name="TextBox 45">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FB49F71-FDF4-423B-BDFD-CFC04E524693}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="1012510">
-            <a:off x="6299969" y="6394450"/>
-            <a:ext cx="699550" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Station C</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>138739</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>142345</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>195434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -954,15 +552,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3682039"/>
-          <a:ext cx="9626600" cy="3686606"/>
+          <a:off x="7429501" y="0"/>
+          <a:ext cx="8439150" cy="3395834"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1252,100 +850,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2020-10-03T17:51:59.675"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1519 3366,'278'0,"-265"1,-1 0,24 7,-22-5,0 0,17 0,415-1,-219-4,-36 2,-177 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2111.37">3124 3385,'1297'0,"-1283"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3690.33">4902 3366,'1175'0,"-1160"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5880.65">6541 3348,'1118'0,"-1104"1,-3 0,25 6,14 2,-36-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8698.84">0 3348,'552'0,"-536"1,-1 0,23 6,-21-3,-1-2,21 2,11-5,-22 0,-2 1,1 1,0 2,24 6,-22-5,1 0,-1-2,0-1,36-3,1 0,4 2,-53 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14544.8">8320 3184,'6'-1,"-1"0,1 0,-1-1,0 0,0 0,0 0,0-1,0 1,0-1,-1 0,2-1,3-6,-3 5,1 0,-1 1,1 0,-1 0,2 0,5-3,21-5,-1-2,60-33,-16 5,39-7,75-35,-172 77,36-11,-36 14,0-2,24-11,-19 6,1 1,0 0,44-9,-54 15,-3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15826.33">9546 2655,'1'-2,"-1"1,1-1,-1 1,1-1,-1 1,1-1,0 1,0-1,0 1,0 0,0-1,0 1,0 0,0 0,1-1,-1 1,0 0,3-1,28-16,-28 15,46-20,52-17,-85 32,103-43,-77 30,1 3,50-14,-51 20,-1-2,-1-3,51-27,-80 37,1 2,0 1,25-5,24-9,143-81,-72 32,-121 62</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17031.64">11013 2016,'0'-1,"0"-1,0 1,0 0,2 0,-2 0,1 0,-1-1,1 1,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,2-1,21-15,-10 9,26-19,69-34,-63 38,52-39,-68 43,2 1,47-20,-44 22,-3 0,35-23,-40 22,48-21,9-6,-32 9,-43 30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18376.25">12152 1342,'11'-1,"2"-2,-2 1,1-1,-1 0,0-1,1 0,-2-1,13-8,-6 4,0 2,26-9,-13 5,0 0,0-3,45-27,36-17,-53 30,68-44,3-4,-117 69,-2 0,2-1,12-11,0-1,-19 16,1 1,0 0,0 0,-1 1,1 0,13-4,-14 5,2-1,0 1,-2-2,2 1,-2-1,1 1,9-7,26-21,-31 25</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20112.79">13464 648,'4'-1,"-1"0,0 0,0 0,0 0,-1-1,1 1,0-1,-1 0,0 1,2-1,-2-2,0 2,3-4,5-3,5-3,0 2,1 0,-1 1,29-12,-26 14,-1-3,1 1,27-21,-24 16,0-1,46-21,-14 7,60-45,25-5,-86 52,-37 20,-1 0,1-2,-2 1,1-1,-2-2,20-16,-24 20,0 0,1 1,-2 1,2-1,0 0,15-4,21-14,-34 17,3-1,-1-2,1 1,18-20,-25 22</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2020-10-03T17:52:26.623"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1,'5'1,"-1"0,1 1,0 0,-2 0,2 0,-1 0,1 2,-2-2,1 1,5 7,3-2,304 225,-222-175,21 13,-83-48,76 49,-11-9,-47-30,69 35,-88-51,35 24,16 10,-26-27,-38-17,1 1,28 18,-26-9,-11-10,-1-1,2 0,-2 0,1 0,0-2,13 5,-20-9,-1 1,0 0,-1-1,1 1,1 0,-1 1,0-1,0 0,1 2,5 6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1441.7">1761 1041,'9'1,"0"1,0 1,0-1,0 1,-1 1,0 0,1 1,-1 0,9 5,10 7,218 100,-213-103,1 1,445 178,-462-188,60 18,89 41,-132-41,-28-18,4 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2595.19">3452 1770,'10'2,"0"-1,0 1,-1 0,0 0,14 6,11 3,103 26,148 41,309 76,-489-124,27 5,-110-31</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4113.38">5333 2281,'7'1,"0"0,-1 0,1 1,-2-1,2 2,-1-1,0 2,6 2,13 6,35 8,-1-4,73 12,-68-15,31 5,6 2,150 48,-6 3,-229-67,5 2,0 1,0 1,22 14,-19-10,12 3,-1-2,57 12,9 3,-86-23</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5566.46">7197 2846,'43'-1,"0"3,0 2,-1 1,49 13,380 92,-176-40,-225-47,-1 3,74 39,-12 3,-110-57,2 0,-1-2,47 11,8 4,-65-20,0-1</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2020-10-03T17:53:30.589"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1485 1097,'2'-133,"-4"-144,1 266,-1 0,-1-2,0 2,0-1,-1 2,-1-1,1 0,-9-11,-14-42,19 46,-1 0,0 2,0-2,-2 3,0-1,-21-22,4 4,12 15,0 1,-1 1,-37-28,-65-35,109 74,-26-16,-4 3,1 0,-1 4,-1 0,0 3,-85-15,83 20,12 0,-1 2,1 2,-57 1,78 5,2-1,-1 1,0 1,1 1,-1-1,2 0,-1 1,0 0,-13 14,11-9,0 0,0 2,2 0,-13 19,-9 13,22-32,-1 0,1 2,1 0,1 0,-1 0,-6 24,-18 96,18-63,-23 130,34-161,2 50,0-56,0 0,-7 53,-6-24,-35 101,-4 48,44-181,-2 31,1-1,3 1,2 65,5-97,2 0,0 0,3 0,10 41,45 112,-47-144,38 85,-31-76,26 78,-36-94,0-2,4 2,-1-2,34 48,0 5,-39-70,0 1,0-1,1-1,1 0,-1 0,2-2,0 2,20 11,7 1,65 33,-96-54,1 0,-2 1,3-2,-3 0,3-1,14 1,-1-2,30-3,-47 2,1 0,-1-1,-1-1,2 1,-2 0,0-1,1 0,-1 0,1 0,7-8,6-6,23-27,-19 19,10-12,42-63,19-23,-77 103,-1-2,-2-2,22-42,-8 14,-19 38,-3-1,1 1,-1-1,-1 0,0-1,-1 1,-2-1,1 0,2-28,1-16,3-15,-7 45,2 0,2 0,0 0,19-52,-15 53,-1 0,-1-1,-2 0,4-49,-1 16,-6 47,3-34,-5 33,2 0,-1-1,3 1,0 0,6-19,-2 10,6-27,-10 32,13-37,-11 44,-3 1,1-1,-2-1,0 1,0-1,1-20,-5-184,1 203</inkml:trace>
-</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1684,7 +1188,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1716,7 +1220,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,22 +1247,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1899,9 +1403,7 @@
       <c r="F6" s="3">
         <v>50</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="12">
         <f t="shared" si="0"/>
@@ -1932,9 +1434,7 @@
       <c r="F7" s="3">
         <v>50</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="12">
         <f t="shared" ref="I7:I16" si="3">E7*D7/100</f>
@@ -2059,7 +1559,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="12">
@@ -2091,9 +1591,7 @@
       <c r="F12" s="3">
         <v>50</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="12">
         <f t="shared" si="3"/>
@@ -2218,7 +1716,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="12">
@@ -2234,26 +1732,14 @@
       <c r="I21" s="17"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
-        <v>1</v>
-      </c>
-      <c r="C25" s="16">
-        <v>2</v>
-      </c>
-      <c r="D25" s="16">
-        <v>3</v>
-      </c>
-      <c r="E25" s="16">
-        <v>4</v>
-      </c>
-      <c r="F25" s="16">
-        <v>5</v>
-      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="A26" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2266,8 +1752,8 @@
   <dimension ref="A1:L154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2304,25 +1790,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2354,7 +1840,7 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2539,10 +2025,10 @@
         <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
@@ -2618,7 +2104,7 @@
         <v>4.125</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2642,7 +2128,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I11" s="12">
         <f t="shared" si="0"/>
@@ -2837,10 +2323,10 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
@@ -3004,10 +2490,10 @@
         <v>55</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
@@ -3141,10 +2627,10 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -3211,7 +2697,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -3403,7 +2889,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="I34" s="12">
         <f t="shared" si="0"/>
@@ -3470,10 +2956,10 @@
         <v>70</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I36" s="12">
         <f t="shared" si="0"/>
@@ -3569,7 +3055,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -3761,7 +3247,7 @@
         <v>70</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="I45" s="12">
         <f t="shared" si="0"/>
@@ -3796,10 +3282,10 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="0"/>
@@ -3863,7 +3349,7 @@
         <v>70</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I48" s="12">
         <f t="shared" si="0"/>
@@ -3895,10 +3381,10 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I49" s="12">
         <f t="shared" si="0"/>
@@ -4017,7 +3503,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -4252,10 +3738,10 @@
         <v>55</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I61" s="12">
         <f t="shared" si="0"/>
@@ -4761,541 +4247,234 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C78" s="5"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="str">
-        <f t="shared" ref="A135:A154" si="6">A134</f>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C154" s="5"/>
     </row>
   </sheetData>
@@ -5309,8 +4488,8 @@
   <dimension ref="A1:N151"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5345,28 +4524,28 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -5401,10 +4580,10 @@
         <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -5428,10 +4607,10 @@
         <v>45</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="1">E3*D3/100</f>
@@ -5449,7 +4628,7 @@
         <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5489,7 +4668,7 @@
         <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -5528,7 +4707,7 @@
         <v>14</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -5567,7 +4746,7 @@
         <v>14</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -5606,7 +4785,7 @@
         <v>14</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5646,7 +4825,7 @@
         <v>14</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5685,7 +4864,7 @@
         <v>14</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -5709,10 +4888,10 @@
         <v>45</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
@@ -5730,7 +4909,7 @@
         <v>14</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5769,7 +4948,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -5808,7 +4987,7 @@
         <v>14</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -5844,10 +5023,10 @@
         <v>8</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -5871,7 +5050,7 @@
         <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
@@ -5886,10 +5065,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5925,10 +5104,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -5964,10 +5143,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -5991,10 +5170,10 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
@@ -6009,10 +5188,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -6048,10 +5227,10 @@
         <v>9</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -6087,10 +5266,10 @@
         <v>9</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -6114,7 +5293,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="1"/>
@@ -6129,10 +5308,10 @@
         <v>9</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6168,10 +5347,10 @@
         <v>9</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6207,10 +5386,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -6234,10 +5413,10 @@
         <v>70</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="1"/>
@@ -6252,10 +5431,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -6291,10 +5470,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -6330,10 +5509,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -6369,10 +5548,10 @@
         <v>10.285714285714286</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6408,10 +5587,10 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -6447,10 +5626,10 @@
         <v>6</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -6486,10 +5665,10 @@
         <v>6</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -6513,7 +5692,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="1"/>
@@ -6528,10 +5707,10 @@
         <v>6</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -6567,10 +5746,10 @@
         <v>6</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -6594,10 +5773,10 @@
         <v>30</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="1"/>
@@ -6615,7 +5794,7 @@
         <v>11</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -6654,7 +5833,7 @@
         <v>11</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -6693,7 +5872,7 @@
         <v>11</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -6732,7 +5911,7 @@
         <v>11</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -6771,7 +5950,7 @@
         <v>11</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -6810,10 +5989,10 @@
         <v>6</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -6855,7 +6034,7 @@
         <v>10</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -6897,7 +6076,7 @@
         <v>10</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -6921,10 +6100,10 @@
         <v>30</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="1"/>
@@ -6942,7 +6121,7 @@
         <v>10</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -6984,7 +6163,7 @@
         <v>10</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -7026,7 +6205,7 @@
         <v>10</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7068,7 +6247,7 @@
         <v>10</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7110,7 +6289,7 @@
         <v>10</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7152,7 +6331,7 @@
         <v>10</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7194,7 +6373,7 @@
         <v>10</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -7236,7 +6415,7 @@
         <v>10</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -7278,7 +6457,7 @@
         <v>10</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -7302,10 +6481,10 @@
         <v>30</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="1"/>
@@ -7323,7 +6502,7 @@
         <v>10</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -7365,7 +6544,7 @@
         <v>10</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -7407,7 +6586,7 @@
         <v>10</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -7449,7 +6628,7 @@
         <v>10</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -7491,7 +6670,7 @@
         <v>10</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -7533,7 +6712,7 @@
         <v>10</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -7575,7 +6754,7 @@
         <v>10</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -7617,7 +6796,7 @@
         <v>10</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -7659,7 +6838,7 @@
         <v>10</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
@@ -7683,10 +6862,10 @@
         <v>30</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="1"/>
@@ -7704,7 +6883,7 @@
         <v>10</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -7741,10 +6920,10 @@
         <v>6</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -7783,7 +6962,7 @@
         <v>0</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -7822,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -7861,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -7898,10 +7077,10 @@
         <v>6</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -7925,7 +7104,7 @@
         <v>70</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I64" s="3">
         <f t="shared" si="1"/>
@@ -7943,7 +7122,7 @@
         <v>1</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -7982,7 +7161,7 @@
         <v>1</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -8006,10 +7185,10 @@
         <v>70</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="1"/>
@@ -8027,7 +7206,7 @@
         <v>1</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -8066,7 +7245,7 @@
         <v>1</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -8105,7 +7284,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -8141,10 +7320,10 @@
         <v>9</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -8183,7 +7362,7 @@
         <v>2</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -8222,7 +7401,7 @@
         <v>2</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -8261,7 +7440,7 @@
         <v>2</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -8300,7 +7479,7 @@
         <v>2</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -8324,10 +7503,10 @@
         <v>40</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="5"/>
@@ -8345,7 +7524,7 @@
         <v>2</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -8384,7 +7563,7 @@
         <v>2</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -8423,7 +7602,7 @@
         <v>2</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -8459,10 +7638,10 @@
         <v>9</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -8486,10 +7665,10 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="8">E78*D78/100</f>
@@ -8504,10 +7683,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -8543,10 +7722,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -8582,10 +7761,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -8621,10 +7800,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -8660,10 +7839,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -8699,10 +7878,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -8738,10 +7917,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -8777,10 +7956,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -8804,7 +7983,7 @@
         <v>70</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I86" s="3">
         <f t="shared" si="8"/>
@@ -8819,10 +7998,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -8858,10 +8037,10 @@
         <v>14.399999999999999</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -8900,7 +8079,7 @@
         <v>5</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -8924,10 +8103,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="8"/>
@@ -8945,7 +8124,7 @@
         <v>5</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -8984,7 +8163,7 @@
         <v>5</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -9023,7 +8202,7 @@
         <v>5</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -9062,7 +8241,7 @@
         <v>5</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -9101,7 +8280,7 @@
         <v>5</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -9140,7 +8319,7 @@
         <v>5</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -9179,7 +8358,7 @@
         <v>5</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -9218,7 +8397,7 @@
         <v>5</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -9242,10 +8421,10 @@
         <v>25</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="8"/>
@@ -9263,7 +8442,7 @@
         <v>5</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -9302,7 +8481,7 @@
         <v>5</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -9341,7 +8520,7 @@
         <v>5</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -9380,7 +8559,7 @@
         <v>5</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -9416,10 +8595,10 @@
         <v>10.799999999999999</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -9455,10 +8634,10 @@
         <v>4.8461538461538467</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -9497,7 +8676,7 @@
         <v>6</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -9536,7 +8715,7 @@
         <v>6</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -9575,7 +8754,7 @@
         <v>6</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -9603,7 +8782,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I106" s="3">
         <f t="shared" si="8"/>
@@ -9621,7 +8800,7 @@
         <v>6</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -9660,7 +8839,7 @@
         <v>6</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -9699,7 +8878,7 @@
         <v>6</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -9738,7 +8917,7 @@
         <v>6</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -9777,7 +8956,7 @@
         <v>6</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -9786,7 +8965,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C111" s="5">
         <v>110</v>
@@ -9813,10 +8992,10 @@
         <v>12</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -9825,7 +9004,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C112" s="3">
         <v>111</v>
@@ -9855,7 +9034,7 @@
         <v>7</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -9864,7 +9043,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C113" s="3">
         <v>112</v>
@@ -9894,7 +9073,7 @@
         <v>7</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -9903,7 +9082,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C114" s="3">
         <v>113</v>
@@ -9933,7 +9112,7 @@
         <v>7</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -9942,7 +9121,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C115" s="5">
         <v>114</v>
@@ -9962,7 +9141,7 @@
         <v>STATION; GLENBURY</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I115" s="3">
         <f t="shared" si="10"/>
@@ -9980,7 +9159,7 @@
         <v>7</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -9989,7 +9168,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C116" s="3">
         <v>115</v>
@@ -10019,7 +9198,7 @@
         <v>7</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -10028,7 +9207,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C117" s="3">
         <v>116</v>
@@ -10058,7 +9237,7 @@
         <v>7</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -10067,7 +9246,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C118" s="3">
         <v>117</v>
@@ -10097,7 +9276,7 @@
         <v>7</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
@@ -10106,7 +9285,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C119" s="5">
         <v>118</v>
@@ -10136,7 +9315,7 @@
         <v>7</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -10145,7 +9324,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C120" s="3">
         <v>119</v>
@@ -10175,7 +9354,7 @@
         <v>7</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -10184,7 +9363,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C121" s="3">
         <v>120</v>
@@ -10214,7 +9393,7 @@
         <v>7</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -10223,7 +9402,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C122" s="3">
         <v>121</v>
@@ -10253,7 +9432,7 @@
         <v>7</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -10262,7 +9441,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C123" s="5">
         <v>122</v>
@@ -10292,10 +9471,10 @@
         <v>9</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -10304,7 +9483,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C124" s="3">
         <v>123</v>
@@ -10319,10 +9498,10 @@
         <v>20</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I124" s="3">
         <f t="shared" si="10"/>
@@ -10340,7 +9519,7 @@
         <v>8</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -10349,7 +9528,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C125" s="3">
         <v>124</v>
@@ -10382,7 +9561,7 @@
         <v>8</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -10391,7 +9570,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C126" s="3">
         <v>125</v>
@@ -10424,7 +9603,7 @@
         <v>8</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -10433,7 +9612,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C127" s="5">
         <v>126</v>
@@ -10466,7 +9645,7 @@
         <v>8</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -10475,7 +9654,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C128" s="3">
         <v>127</v>
@@ -10508,7 +9687,7 @@
         <v>8</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -10517,7 +9696,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C129" s="3">
         <v>128</v>
@@ -10550,7 +9729,7 @@
         <v>8</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
@@ -10559,7 +9738,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C130" s="3">
         <v>129</v>
@@ -10592,7 +9771,7 @@
         <v>8</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -10601,7 +9780,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C131" s="5">
         <v>130</v>
@@ -10634,7 +9813,7 @@
         <v>8</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -10643,7 +9822,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C132" s="3">
         <v>131</v>
@@ -10676,7 +9855,7 @@
         <v>8</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -10685,7 +9864,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C133" s="3">
         <v>132</v>
@@ -10704,7 +9883,7 @@
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I133" s="3">
         <f t="shared" si="10"/>
@@ -10722,7 +9901,7 @@
         <v>8</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
@@ -10731,7 +9910,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C134" s="3">
         <v>133</v>
@@ -10764,7 +9943,7 @@
         <v>8</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -10773,7 +9952,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C135" s="5">
         <v>134</v>
@@ -10806,7 +9985,7 @@
         <v>8</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -10815,7 +9994,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C136" s="3">
         <v>135</v>
@@ -10848,7 +10027,7 @@
         <v>8</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -10857,7 +10036,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C137" s="3">
         <v>136</v>
@@ -10890,7 +10069,7 @@
         <v>8</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -10899,7 +10078,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C138" s="3">
         <v>137</v>
@@ -10932,7 +10111,7 @@
         <v>8</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -10941,7 +10120,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C139" s="5">
         <v>138</v>
@@ -10974,7 +10153,7 @@
         <v>8</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -10983,7 +10162,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C140" s="3">
         <v>139</v>
@@ -11016,7 +10195,7 @@
         <v>8</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -11025,7 +10204,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C141" s="3">
         <v>140</v>
@@ -11058,7 +10237,7 @@
         <v>8</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -11067,7 +10246,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C142" s="3">
         <v>141</v>
@@ -11086,7 +10265,7 @@
         <v>STATION; CENTRAL; UNDERDROUND</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I142" s="3">
         <f t="shared" si="10"/>
@@ -11104,7 +10283,7 @@
         <v>8</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
@@ -11113,7 +10292,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C143" s="5">
         <v>142</v>
@@ -11146,7 +10325,7 @@
         <v>8</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -11155,7 +10334,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C144" s="3">
         <v>143</v>
@@ -11188,7 +10367,7 @@
         <v>8</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -11197,7 +10376,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C145" s="3">
         <v>144</v>
@@ -11224,10 +10403,10 @@
         <v>9</v>
       </c>
       <c r="M145" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -11236,7 +10415,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C146" s="3">
         <v>145</v>
@@ -11266,7 +10445,7 @@
         <v>9</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -11275,7 +10454,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C147" s="5">
         <v>146</v>
@@ -11305,7 +10484,7 @@
         <v>9</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -11314,7 +10493,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C148" s="3">
         <v>147</v>
@@ -11344,7 +10523,7 @@
         <v>9</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -11353,7 +10532,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C149" s="3">
         <v>148</v>
@@ -11384,7 +10563,7 @@
         <v>9</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -11393,7 +10572,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C150" s="3">
         <v>149</v>
@@ -11423,7 +10602,7 @@
         <v>9</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -11432,7 +10611,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C151" s="5">
         <v>150</v>
@@ -11459,10 +10638,10 @@
         <v>6.3</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issues in track model
</commit_message>
<xml_diff>
--- a/TrackModelV2/track.xlsx
+++ b/TrackModelV2/track.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himes\ECE1140\ECE1140\TrackModelV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8980DB8-A3D5-48F5-AED5-A4F1FB2A1726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FCDDA8-C0EF-49C5-937A-45D632BED0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="105" windowWidth="27780" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
     <sheet name="Blue Line" sheetId="7" r:id="rId2"/>
-    <sheet name="Red Line" sheetId="1" r:id="rId3"/>
-    <sheet name="Green Line" sheetId="2" r:id="rId4"/>
+    <sheet name="Red Line!" sheetId="1" r:id="rId3"/>
+    <sheet name="Green Line!" sheetId="2" r:id="rId4"/>
     <sheet name="Track Layout" sheetId="4" r:id="rId5"/>
     <sheet name="Vehicle Data 1" sheetId="5" r:id="rId6"/>
     <sheet name="Vehicle Data 2" sheetId="6" r:id="rId7"/>
@@ -4024,7 +4024,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="str">
-        <f t="shared" ref="A71:A134" si="5">A70</f>
+        <f t="shared" ref="A71:A77" si="5">A70</f>
         <v>Red</v>
       </c>
       <c r="B71" s="3" t="s">

</xml_diff>

<commit_message>
fixed excel and commented out block_table code that lags the whole simulation
</commit_message>
<xml_diff>
--- a/TrackModelV2/track.xlsx
+++ b/TrackModelV2/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himes\ECE1140\ECE1140\TrackModelV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FCDDA8-C0EF-49C5-937A-45D632BED0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF420D2-8C89-4616-9346-65FA4AD0876F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="105" windowWidth="27780" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="255" windowWidth="27780" windowHeight="14625" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -22,14 +22,6 @@
     <sheet name="Vehicle Data 2" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1751,9 +1743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4485,11 +4477,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N151"/>
+  <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4507,7 +4499,7 @@
     <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -4538,17 +4530,18 @@
       <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -4575,18 +4568,19 @@
         <f>I2</f>
         <v>0.5</v>
       </c>
-      <c r="K2" s="15">
-        <f t="shared" ref="K2:K65" si="0">D2*(1/(F2*1000/(60*60)))</f>
+      <c r="K2" s="3"/>
+      <c r="L2" s="15">
+        <f t="shared" ref="L2:L65" si="0">D2*(1/(F2*1000/(60*60)))</f>
         <v>8</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -4620,18 +4614,19 @@
         <f>I3+J2</f>
         <v>1.5</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="3"/>
+      <c r="L3" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>14</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="2">A3</f>
         <v>Green</v>
@@ -4659,19 +4654,20 @@
         <f t="shared" ref="J4:J67" si="3">I4+J3</f>
         <v>3</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="3"/>
+      <c r="L4" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="1">
+      <c r="M4" s="9"/>
+      <c r="N4" s="1">
         <v>14</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4699,18 +4695,19 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="3"/>
+      <c r="L5" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>14</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4738,18 +4735,19 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="3"/>
+      <c r="L6" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>14</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4777,18 +4775,19 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="3"/>
+      <c r="L7" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>14</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4817,18 +4816,19 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="3"/>
+      <c r="L8" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>14</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4856,18 +4856,19 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="3"/>
+      <c r="L9" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>14</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4901,18 +4902,19 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="3"/>
+      <c r="L10" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>14</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4940,18 +4942,19 @@
         <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="3"/>
+      <c r="L11" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>14</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4979,18 +4982,19 @@
         <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="3"/>
+      <c r="L12" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>14</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5018,18 +5022,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="3"/>
+      <c r="L13" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5060,18 +5065,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="3"/>
+      <c r="L14" s="15">
         <f t="shared" si="0"/>
         <v>7.7142857142857153</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5099,18 +5105,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="3"/>
+      <c r="L15" s="15">
         <f t="shared" si="0"/>
         <v>7.7142857142857153</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5138,18 +5145,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="3"/>
+      <c r="L16" s="15">
         <f t="shared" si="0"/>
         <v>7.7142857142857153</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5183,18 +5191,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="3"/>
+      <c r="L17" s="15">
         <f t="shared" si="0"/>
         <v>7.7142857142857153</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5222,18 +5231,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="3"/>
+      <c r="L18" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5261,18 +5271,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="3"/>
+      <c r="L19" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5303,18 +5314,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K20" s="3"/>
+      <c r="L20" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5342,18 +5354,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="3"/>
+      <c r="L21" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5381,18 +5394,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K22" s="15">
+      <c r="K22" s="3"/>
+      <c r="L22" s="15">
         <f t="shared" si="0"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5426,18 +5440,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K23" s="15">
+      <c r="K23" s="3"/>
+      <c r="L23" s="15">
         <f t="shared" si="0"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5465,18 +5480,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="3"/>
+      <c r="L24" s="15">
         <f t="shared" si="0"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5504,18 +5520,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="3"/>
+      <c r="L25" s="15">
         <f t="shared" si="0"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5543,18 +5560,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="3"/>
+      <c r="L26" s="15">
         <f t="shared" si="0"/>
         <v>10.285714285714286</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5582,18 +5600,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K27" s="15">
+      <c r="K27" s="3"/>
+      <c r="L27" s="15">
         <f t="shared" si="0"/>
         <v>5.1428571428571432</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5621,18 +5640,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K28" s="15">
+      <c r="K28" s="3"/>
+      <c r="L28" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5660,18 +5680,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="3"/>
+      <c r="L29" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5702,18 +5723,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K30" s="15">
+      <c r="K30" s="3"/>
+      <c r="L30" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N30" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5741,18 +5763,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="3"/>
+      <c r="L31" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5786,18 +5809,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="3"/>
+      <c r="L32" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <v>11</v>
       </c>
-      <c r="N32" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5825,18 +5849,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K33" s="15">
+      <c r="K33" s="3"/>
+      <c r="L33" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>11</v>
       </c>
-      <c r="N33" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5864,18 +5889,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K34" s="15">
+      <c r="K34" s="3"/>
+      <c r="L34" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <v>11</v>
       </c>
-      <c r="N34" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5903,18 +5929,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K35" s="15">
+      <c r="K35" s="3"/>
+      <c r="L35" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>11</v>
       </c>
-      <c r="N35" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5942,18 +5969,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="3"/>
+      <c r="L36" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M36" s="1">
+      <c r="N36" s="1">
         <v>11</v>
       </c>
-      <c r="N36" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5984,18 +6012,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="3"/>
+      <c r="L37" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -6026,18 +6055,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K38" s="15">
+      <c r="K38" s="3"/>
+      <c r="L38" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M38" s="1">
+      <c r="N38" s="1">
         <v>10</v>
       </c>
-      <c r="N38" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6068,18 +6098,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K39" s="15">
+      <c r="K39" s="3"/>
+      <c r="L39" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M39" s="1">
+      <c r="N39" s="1">
         <v>10</v>
       </c>
-      <c r="N39" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="O39" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6113,18 +6144,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K40" s="15">
+      <c r="K40" s="3"/>
+      <c r="L40" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M40" s="1">
+      <c r="N40" s="1">
         <v>10</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6155,18 +6187,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K41" s="15">
+      <c r="K41" s="3"/>
+      <c r="L41" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M41" s="1">
+      <c r="N41" s="1">
         <v>10</v>
       </c>
-      <c r="N41" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6197,18 +6230,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K42" s="15">
+      <c r="K42" s="3"/>
+      <c r="L42" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M42" s="1">
+      <c r="N42" s="1">
         <v>10</v>
       </c>
-      <c r="N42" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6239,18 +6273,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K43" s="15">
+      <c r="K43" s="3"/>
+      <c r="L43" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M43" s="1">
+      <c r="N43" s="1">
         <v>10</v>
       </c>
-      <c r="N43" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6281,18 +6316,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K44" s="15">
+      <c r="K44" s="3"/>
+      <c r="L44" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M44" s="1">
+      <c r="N44" s="1">
         <v>10</v>
       </c>
-      <c r="N44" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6323,18 +6359,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K45" s="15">
+      <c r="K45" s="3"/>
+      <c r="L45" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M45" s="1">
+      <c r="N45" s="1">
         <v>10</v>
       </c>
-      <c r="N45" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6365,18 +6402,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K46" s="15">
+      <c r="K46" s="3"/>
+      <c r="L46" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M46" s="1">
+      <c r="N46" s="1">
         <v>10</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6407,18 +6445,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K47" s="15">
+      <c r="K47" s="3"/>
+      <c r="L47" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M47" s="1">
+      <c r="N47" s="1">
         <v>10</v>
       </c>
-      <c r="N47" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6449,18 +6488,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K48" s="15">
+      <c r="K48" s="3"/>
+      <c r="L48" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M48" s="1">
+      <c r="N48" s="1">
         <v>10</v>
       </c>
-      <c r="N48" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="O48" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6494,18 +6534,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K49" s="15">
+      <c r="K49" s="3"/>
+      <c r="L49" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M49" s="1">
+      <c r="N49" s="1">
         <v>10</v>
       </c>
-      <c r="N49" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6536,18 +6577,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K50" s="15">
+      <c r="K50" s="3"/>
+      <c r="L50" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M50" s="1">
+      <c r="N50" s="1">
         <v>10</v>
       </c>
-      <c r="N50" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6578,18 +6620,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K51" s="15">
+      <c r="K51" s="3"/>
+      <c r="L51" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M51" s="1">
+      <c r="N51" s="1">
         <v>10</v>
       </c>
-      <c r="N51" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6620,18 +6663,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K52" s="15">
+      <c r="K52" s="3"/>
+      <c r="L52" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M52" s="1">
+      <c r="N52" s="1">
         <v>10</v>
       </c>
-      <c r="N52" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6662,18 +6706,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K53" s="15">
+      <c r="K53" s="3"/>
+      <c r="L53" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M53" s="1">
+      <c r="N53" s="1">
         <v>10</v>
       </c>
-      <c r="N53" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6704,18 +6749,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K54" s="15">
+      <c r="K54" s="3"/>
+      <c r="L54" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M54" s="1">
+      <c r="N54" s="1">
         <v>10</v>
       </c>
-      <c r="N54" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6746,18 +6792,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K55" s="15">
+      <c r="K55" s="3"/>
+      <c r="L55" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M55" s="1">
+      <c r="N55" s="1">
         <v>10</v>
       </c>
-      <c r="N55" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6788,18 +6835,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K56" s="15">
+      <c r="K56" s="3"/>
+      <c r="L56" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M56" s="1">
+      <c r="N56" s="1">
         <v>10</v>
       </c>
-      <c r="N56" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6830,18 +6878,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K57" s="15">
+      <c r="K57" s="3"/>
+      <c r="L57" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M57" s="1">
+      <c r="N57" s="1">
         <v>10</v>
       </c>
-      <c r="N57" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="O57" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6875,18 +6924,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K58" s="15">
+      <c r="K58" s="3"/>
+      <c r="L58" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M58" s="1">
+      <c r="N58" s="1">
         <v>10</v>
       </c>
-      <c r="N58" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6915,18 +6965,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K59" s="15">
+      <c r="K59" s="3"/>
+      <c r="L59" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M59" s="1" t="s">
+      <c r="N59" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N59" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6954,18 +7005,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K60" s="15">
+      <c r="K60" s="3"/>
+      <c r="L60" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M60" s="1">
-        <v>0</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N60" s="1">
+        <v>0</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6993,18 +7045,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K61" s="15">
+      <c r="K61" s="3"/>
+      <c r="L61" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M61" s="1">
-        <v>0</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N61" s="1">
+        <v>0</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7032,18 +7085,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K62" s="15">
+      <c r="K62" s="3"/>
+      <c r="L62" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M62" s="1">
-        <v>0</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N62" s="1">
+        <v>0</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7072,18 +7126,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K63" s="15">
+      <c r="K63" s="3"/>
+      <c r="L63" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="N63" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N63" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7114,18 +7169,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K64" s="15">
+      <c r="K64" s="3"/>
+      <c r="L64" s="15">
         <f t="shared" si="0"/>
         <v>5.1428571428571432</v>
       </c>
-      <c r="M64" s="1">
+      <c r="N64" s="1">
         <v>1</v>
       </c>
-      <c r="N64" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7153,18 +7209,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K65" s="15">
+      <c r="K65" s="3"/>
+      <c r="L65" s="15">
         <f t="shared" si="0"/>
         <v>5.1428571428571432</v>
       </c>
-      <c r="M65" s="1">
+      <c r="N65" s="1">
         <v>1</v>
       </c>
-      <c r="N65" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7198,18 +7255,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K66" s="15">
-        <f t="shared" ref="K66:K129" si="4">D66*(1/(F66*1000/(60*60)))</f>
+      <c r="K66" s="3"/>
+      <c r="L66" s="15">
+        <f t="shared" ref="L66:L129" si="4">D66*(1/(F66*1000/(60*60)))</f>
         <v>10.285714285714286</v>
       </c>
-      <c r="M66" s="1">
+      <c r="N66" s="1">
         <v>1</v>
       </c>
-      <c r="N66" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7237,18 +7295,19 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K67" s="15">
+      <c r="K67" s="3"/>
+      <c r="L67" s="15">
         <f t="shared" si="4"/>
         <v>10.285714285714286</v>
       </c>
-      <c r="M67" s="1">
+      <c r="N67" s="1">
         <v>1</v>
       </c>
-      <c r="N67" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7276,18 +7335,19 @@
         <f t="shared" ref="J68:J77" si="6">I68+J67</f>
         <v>0.5</v>
       </c>
-      <c r="K68" s="15">
+      <c r="K68" s="3"/>
+      <c r="L68" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M68" s="1">
+      <c r="N68" s="1">
         <v>1</v>
       </c>
-      <c r="N68" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7315,18 +7375,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K69" s="15">
+      <c r="K69" s="3"/>
+      <c r="L69" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="N69" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N69" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7354,18 +7415,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K70" s="15">
+      <c r="K70" s="3"/>
+      <c r="L70" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M70" s="1">
+      <c r="N70" s="1">
         <v>2</v>
       </c>
-      <c r="N70" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A134" si="7">A70</f>
         <v>Green</v>
@@ -7393,18 +7455,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K71" s="15">
+      <c r="K71" s="3"/>
+      <c r="L71" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M71" s="1">
+      <c r="N71" s="1">
         <v>2</v>
       </c>
-      <c r="N71" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7432,18 +7495,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K72" s="15">
+      <c r="K72" s="3"/>
+      <c r="L72" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M72" s="1">
+      <c r="N72" s="1">
         <v>2</v>
       </c>
-      <c r="N72" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7471,18 +7535,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K73" s="15">
+      <c r="K73" s="3"/>
+      <c r="L73" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M73" s="1">
+      <c r="N73" s="1">
         <v>2</v>
       </c>
-      <c r="N73" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7516,18 +7581,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K74" s="15">
+      <c r="K74" s="3"/>
+      <c r="L74" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M74" s="1">
+      <c r="N74" s="1">
         <v>2</v>
       </c>
-      <c r="N74" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7555,18 +7621,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K75" s="15">
+      <c r="K75" s="3"/>
+      <c r="L75" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M75" s="1">
+      <c r="N75" s="1">
         <v>2</v>
       </c>
-      <c r="N75" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7594,18 +7661,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K76" s="15">
+      <c r="K76" s="3"/>
+      <c r="L76" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M76" s="1">
+      <c r="N76" s="1">
         <v>2</v>
       </c>
-      <c r="N76" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7633,18 +7701,19 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="K77" s="15">
+      <c r="K77" s="3"/>
+      <c r="L77" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M77" s="1" t="s">
+      <c r="N77" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N77" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="O77" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7678,18 +7747,19 @@
         <f t="shared" ref="J78:J109" si="9">I78+J77</f>
         <v>0.5</v>
       </c>
-      <c r="K78" s="15">
+      <c r="K78" s="3"/>
+      <c r="L78" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M78" s="1" t="s">
+      <c r="N78" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N78" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7717,18 +7787,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K79" s="15">
+      <c r="K79" s="3"/>
+      <c r="L79" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M79" s="1" t="s">
+      <c r="N79" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N79" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7756,18 +7827,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K80" s="15">
+      <c r="K80" s="3"/>
+      <c r="L80" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M80" s="1" t="s">
+      <c r="N80" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N80" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7795,18 +7867,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K81" s="15">
+      <c r="K81" s="3"/>
+      <c r="L81" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="N81" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N81" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7834,18 +7907,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K82" s="15">
+      <c r="K82" s="3"/>
+      <c r="L82" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M82" s="1" t="s">
+      <c r="N82" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N82" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7873,18 +7947,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K83" s="15">
+      <c r="K83" s="3"/>
+      <c r="L83" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M83" s="1" t="s">
+      <c r="N83" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N83" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7912,18 +7987,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K84" s="15">
+      <c r="K84" s="3"/>
+      <c r="L84" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M84" s="1" t="s">
+      <c r="N84" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N84" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7951,18 +8027,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K85" s="15">
+      <c r="K85" s="3"/>
+      <c r="L85" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M85" s="1" t="s">
+      <c r="N85" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N85" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7993,18 +8070,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K86" s="15">
+      <c r="K86" s="3"/>
+      <c r="L86" s="15">
         <f t="shared" si="4"/>
         <v>15.428571428571431</v>
       </c>
-      <c r="M86" s="1" t="s">
+      <c r="N86" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="N86" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8032,18 +8110,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K87" s="15">
+      <c r="K87" s="3"/>
+      <c r="L87" s="15">
         <f t="shared" si="4"/>
         <v>14.399999999999999</v>
       </c>
-      <c r="M87" s="1" t="s">
+      <c r="N87" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N87" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8071,18 +8150,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K88" s="15">
+      <c r="K88" s="3"/>
+      <c r="L88" s="15">
         <f t="shared" si="4"/>
         <v>12.470399999999998</v>
       </c>
-      <c r="M88" s="1">
+      <c r="N88" s="1">
         <v>5</v>
       </c>
-      <c r="N88" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8116,18 +8196,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K89" s="15">
+      <c r="K89" s="3"/>
+      <c r="L89" s="15">
         <f t="shared" si="4"/>
         <v>14.399999999999999</v>
       </c>
-      <c r="M89" s="1">
+      <c r="N89" s="1">
         <v>5</v>
       </c>
-      <c r="N89" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8155,18 +8236,19 @@
         <f t="shared" si="9"/>
         <v>0.125</v>
       </c>
-      <c r="K90" s="15">
+      <c r="K90" s="3"/>
+      <c r="L90" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M90" s="1">
+      <c r="N90" s="1">
         <v>5</v>
       </c>
-      <c r="N90" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8194,18 +8276,19 @@
         <f t="shared" si="9"/>
         <v>-0.625</v>
       </c>
-      <c r="K91" s="15">
+      <c r="K91" s="3"/>
+      <c r="L91" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M91" s="1">
+      <c r="N91" s="1">
         <v>5</v>
       </c>
-      <c r="N91" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8233,18 +8316,19 @@
         <f t="shared" si="9"/>
         <v>-2.125</v>
       </c>
-      <c r="K92" s="15">
+      <c r="K92" s="3"/>
+      <c r="L92" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M92" s="1">
+      <c r="N92" s="1">
         <v>5</v>
       </c>
-      <c r="N92" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8272,18 +8356,19 @@
         <f t="shared" si="9"/>
         <v>-2.125</v>
       </c>
-      <c r="K93" s="15">
+      <c r="K93" s="3"/>
+      <c r="L93" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M93" s="1">
+      <c r="N93" s="1">
         <v>5</v>
       </c>
-      <c r="N93" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8311,18 +8396,19 @@
         <f t="shared" si="9"/>
         <v>-0.625</v>
       </c>
-      <c r="K94" s="15">
+      <c r="K94" s="3"/>
+      <c r="L94" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M94" s="1">
+      <c r="N94" s="1">
         <v>5</v>
       </c>
-      <c r="N94" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8350,18 +8436,19 @@
         <f t="shared" si="9"/>
         <v>0.125</v>
       </c>
-      <c r="K95" s="15">
+      <c r="K95" s="3"/>
+      <c r="L95" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M95" s="1">
+      <c r="N95" s="1">
         <v>5</v>
       </c>
-      <c r="N95" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8389,18 +8476,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K96" s="15">
+      <c r="K96" s="3"/>
+      <c r="L96" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M96" s="1">
+      <c r="N96" s="1">
         <v>5</v>
       </c>
-      <c r="N96" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8434,18 +8522,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K97" s="15">
+      <c r="K97" s="3"/>
+      <c r="L97" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M97" s="1">
+      <c r="N97" s="1">
         <v>5</v>
       </c>
-      <c r="N97" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8473,18 +8562,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K98" s="15">
+      <c r="K98" s="3"/>
+      <c r="L98" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M98" s="1">
+      <c r="N98" s="1">
         <v>5</v>
       </c>
-      <c r="N98" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8512,18 +8602,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K99" s="15">
+      <c r="K99" s="3"/>
+      <c r="L99" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M99" s="1">
+      <c r="N99" s="1">
         <v>5</v>
       </c>
-      <c r="N99" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8551,18 +8642,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K100" s="15">
+      <c r="K100" s="3"/>
+      <c r="L100" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M100" s="1">
+      <c r="N100" s="1">
         <v>5</v>
       </c>
-      <c r="N100" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8590,18 +8682,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K101" s="15">
+      <c r="K101" s="3"/>
+      <c r="L101" s="15">
         <f t="shared" si="4"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="M101" s="1" t="s">
+      <c r="N101" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N101" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8629,18 +8722,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K102" s="15">
+      <c r="K102" s="3"/>
+      <c r="L102" s="15">
         <f t="shared" si="4"/>
         <v>4.8461538461538467</v>
       </c>
-      <c r="M102" s="1" t="s">
+      <c r="N102" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N102" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8668,18 +8762,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K103" s="15">
+      <c r="K103" s="3"/>
+      <c r="L103" s="15">
         <f t="shared" si="4"/>
         <v>12.857142857142859</v>
       </c>
-      <c r="M103" s="1">
+      <c r="N103" s="1">
         <v>6</v>
       </c>
-      <c r="N103" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8707,18 +8802,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K104" s="15">
+      <c r="K104" s="3"/>
+      <c r="L104" s="15">
         <f t="shared" si="4"/>
         <v>12.857142857142859</v>
       </c>
-      <c r="M104" s="1">
+      <c r="N104" s="1">
         <v>6</v>
       </c>
-      <c r="N104" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8746,18 +8842,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K105" s="15">
+      <c r="K105" s="3"/>
+      <c r="L105" s="15">
         <f t="shared" si="4"/>
         <v>10.285714285714286</v>
       </c>
-      <c r="M105" s="1">
+      <c r="N105" s="1">
         <v>6</v>
       </c>
-      <c r="N105" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8792,18 +8889,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K106" s="15">
+      <c r="K106" s="3"/>
+      <c r="L106" s="15">
         <f t="shared" si="4"/>
         <v>12.857142857142859</v>
       </c>
-      <c r="M106" s="1">
+      <c r="N106" s="1">
         <v>6</v>
       </c>
-      <c r="N106" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8831,18 +8929,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K107" s="15">
+      <c r="K107" s="3"/>
+      <c r="L107" s="15">
         <f t="shared" si="4"/>
         <v>12.857142857142859</v>
       </c>
-      <c r="M107" s="1">
+      <c r="N107" s="1">
         <v>6</v>
       </c>
-      <c r="N107" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8870,18 +8969,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K108" s="15">
+      <c r="K108" s="3"/>
+      <c r="L108" s="15">
         <f t="shared" si="4"/>
         <v>11.571428571428573</v>
       </c>
-      <c r="M108" s="1">
+      <c r="N108" s="1">
         <v>6</v>
       </c>
-      <c r="N108" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8909,18 +9009,19 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K109" s="15">
+      <c r="K109" s="3"/>
+      <c r="L109" s="15">
         <f t="shared" si="4"/>
         <v>12.857142857142859</v>
       </c>
-      <c r="M109" s="1">
+      <c r="N109" s="1">
         <v>6</v>
       </c>
-      <c r="N109" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O109" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8948,18 +9049,19 @@
         <f t="shared" ref="J110:J151" si="11">I110+J109</f>
         <v>0.5</v>
       </c>
-      <c r="K110" s="15">
+      <c r="K110" s="3"/>
+      <c r="L110" s="15">
         <f t="shared" si="4"/>
         <v>12.857142857142859</v>
       </c>
-      <c r="M110" s="1">
+      <c r="N110" s="1">
         <v>6</v>
       </c>
-      <c r="N110" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O110" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8987,18 +9089,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K111" s="15">
+      <c r="K111" s="3"/>
+      <c r="L111" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M111" s="1" t="s">
+      <c r="N111" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N111" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O111" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9026,18 +9129,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K112" s="15">
+      <c r="K112" s="3"/>
+      <c r="L112" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M112" s="1">
+      <c r="N112" s="1">
         <v>7</v>
       </c>
-      <c r="N112" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O112" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9065,18 +9169,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K113" s="15">
+      <c r="K113" s="3"/>
+      <c r="L113" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M113" s="1">
+      <c r="N113" s="1">
         <v>7</v>
       </c>
-      <c r="N113" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9104,18 +9209,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K114" s="15">
+      <c r="K114" s="3"/>
+      <c r="L114" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M114" s="1">
+      <c r="N114" s="1">
         <v>7</v>
       </c>
-      <c r="N114" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9151,18 +9257,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K115" s="15">
+      <c r="K115" s="3"/>
+      <c r="L115" s="15">
         <f t="shared" si="4"/>
         <v>19.439999999999998</v>
       </c>
-      <c r="M115" s="1">
+      <c r="N115" s="1">
         <v>7</v>
       </c>
-      <c r="N115" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O115" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9190,18 +9297,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K116" s="15">
+      <c r="K116" s="3"/>
+      <c r="L116" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M116" s="1">
+      <c r="N116" s="1">
         <v>7</v>
       </c>
-      <c r="N116" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O116" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9229,18 +9337,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K117" s="15">
+      <c r="K117" s="3"/>
+      <c r="L117" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M117" s="1">
+      <c r="N117" s="1">
         <v>7</v>
       </c>
-      <c r="N117" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9268,18 +9377,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K118" s="15">
+      <c r="K118" s="3"/>
+      <c r="L118" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M118" s="1">
+      <c r="N118" s="1">
         <v>7</v>
       </c>
-      <c r="N118" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9307,18 +9417,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K119" s="15">
+      <c r="K119" s="3"/>
+      <c r="L119" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M119" s="1">
+      <c r="N119" s="1">
         <v>7</v>
       </c>
-      <c r="N119" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O119" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9346,18 +9457,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K120" s="15">
+      <c r="K120" s="3"/>
+      <c r="L120" s="15">
         <f t="shared" si="4"/>
         <v>9.6</v>
       </c>
-      <c r="M120" s="1">
+      <c r="N120" s="1">
         <v>7</v>
       </c>
-      <c r="N120" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9385,18 +9497,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K121" s="15">
+      <c r="K121" s="3"/>
+      <c r="L121" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M121" s="1">
+      <c r="N121" s="1">
         <v>7</v>
       </c>
-      <c r="N121" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9424,18 +9537,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K122" s="15">
+      <c r="K122" s="3"/>
+      <c r="L122" s="15">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="M122" s="1">
+      <c r="N122" s="1">
         <v>7</v>
       </c>
-      <c r="N122" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9466,18 +9580,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K123" s="15">
+      <c r="K123" s="3"/>
+      <c r="L123" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M123" s="1" t="s">
+      <c r="N123" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N123" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="124" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="O123" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9511,18 +9626,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K124" s="15">
+      <c r="K124" s="3"/>
+      <c r="L124" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M124" s="1">
+      <c r="N124" s="1">
         <v>8</v>
       </c>
-      <c r="N124" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O124" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9553,18 +9669,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K125" s="15">
+      <c r="K125" s="3"/>
+      <c r="L125" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M125" s="1">
+      <c r="N125" s="1">
         <v>8</v>
       </c>
-      <c r="N125" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O125" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9595,18 +9712,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K126" s="15">
+      <c r="K126" s="3"/>
+      <c r="L126" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M126" s="1">
+      <c r="N126" s="1">
         <v>8</v>
       </c>
-      <c r="N126" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O126" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9637,18 +9755,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K127" s="15">
+      <c r="K127" s="3"/>
+      <c r="L127" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M127" s="1">
+      <c r="N127" s="1">
         <v>8</v>
       </c>
-      <c r="N127" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O127" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9679,18 +9798,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K128" s="15">
+      <c r="K128" s="3"/>
+      <c r="L128" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M128" s="1">
+      <c r="N128" s="1">
         <v>8</v>
       </c>
-      <c r="N128" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O128" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9721,18 +9841,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K129" s="15">
+      <c r="K129" s="3"/>
+      <c r="L129" s="15">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="M129" s="1">
+      <c r="N129" s="1">
         <v>8</v>
       </c>
-      <c r="N129" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O129" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9763,18 +9884,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K130" s="15">
-        <f t="shared" ref="K130:K150" si="12">D130*(1/(F130*1000/(60*60)))</f>
+      <c r="K130" s="3"/>
+      <c r="L130" s="15">
+        <f t="shared" ref="L130:L150" si="12">D130*(1/(F130*1000/(60*60)))</f>
         <v>9</v>
       </c>
-      <c r="M130" s="1">
+      <c r="N130" s="1">
         <v>8</v>
       </c>
-      <c r="N130" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O130" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9805,18 +9927,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K131" s="15">
+      <c r="K131" s="3"/>
+      <c r="L131" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M131" s="1">
+      <c r="N131" s="1">
         <v>8</v>
       </c>
-      <c r="N131" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O131" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9847,18 +9970,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K132" s="15">
+      <c r="K132" s="3"/>
+      <c r="L132" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M132" s="1">
+      <c r="N132" s="1">
         <v>8</v>
       </c>
-      <c r="N132" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="133" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="O132" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9893,18 +10017,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K133" s="15">
+      <c r="K133" s="3"/>
+      <c r="L133" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M133" s="1">
+      <c r="N133" s="1">
         <v>8</v>
       </c>
-      <c r="N133" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O133" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9935,18 +10060,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K134" s="15">
+      <c r="K134" s="3"/>
+      <c r="L134" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M134" s="1">
+      <c r="N134" s="1">
         <v>8</v>
       </c>
-      <c r="N134" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O134" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="str">
         <f t="shared" ref="A135:A151" si="13">A134</f>
         <v>Green</v>
@@ -9977,18 +10103,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K135" s="15">
+      <c r="K135" s="3"/>
+      <c r="L135" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M135" s="1">
+      <c r="N135" s="1">
         <v>8</v>
       </c>
-      <c r="N135" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O135" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10019,18 +10146,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K136" s="15">
+      <c r="K136" s="3"/>
+      <c r="L136" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M136" s="1">
+      <c r="N136" s="1">
         <v>8</v>
       </c>
-      <c r="N136" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O136" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10061,18 +10189,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K137" s="15">
+      <c r="K137" s="3"/>
+      <c r="L137" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M137" s="1">
+      <c r="N137" s="1">
         <v>8</v>
       </c>
-      <c r="N137" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O137" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10103,18 +10232,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K138" s="15">
+      <c r="K138" s="3"/>
+      <c r="L138" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M138" s="1">
+      <c r="N138" s="1">
         <v>8</v>
       </c>
-      <c r="N138" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O138" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10145,18 +10275,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K139" s="15">
+      <c r="K139" s="3"/>
+      <c r="L139" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M139" s="1">
+      <c r="N139" s="1">
         <v>8</v>
       </c>
-      <c r="N139" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O139" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10187,18 +10318,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K140" s="15">
+      <c r="K140" s="3"/>
+      <c r="L140" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M140" s="1">
+      <c r="N140" s="1">
         <v>8</v>
       </c>
-      <c r="N140" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O140" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10229,18 +10361,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K141" s="15">
+      <c r="K141" s="3"/>
+      <c r="L141" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M141" s="1">
+      <c r="N141" s="1">
         <v>8</v>
       </c>
-      <c r="N141" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="O141" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10275,18 +10408,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K142" s="15">
+      <c r="K142" s="3"/>
+      <c r="L142" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M142" s="1">
+      <c r="N142" s="1">
         <v>8</v>
       </c>
-      <c r="N142" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O142" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10317,18 +10451,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K143" s="15">
+      <c r="K143" s="3"/>
+      <c r="L143" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M143" s="1">
+      <c r="N143" s="1">
         <v>8</v>
       </c>
-      <c r="N143" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O143" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10359,18 +10494,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K144" s="15">
+      <c r="K144" s="3"/>
+      <c r="L144" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M144" s="1">
+      <c r="N144" s="1">
         <v>8</v>
       </c>
-      <c r="N144" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O144" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10398,18 +10534,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K145" s="15">
+      <c r="K145" s="3"/>
+      <c r="L145" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M145" s="1" t="s">
+      <c r="N145" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N145" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O145" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10437,18 +10574,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K146" s="15">
+      <c r="K146" s="3"/>
+      <c r="L146" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M146" s="1">
+      <c r="N146" s="1">
         <v>9</v>
       </c>
-      <c r="N146" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O146" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10476,18 +10614,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K147" s="15">
+      <c r="K147" s="3"/>
+      <c r="L147" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M147" s="1">
+      <c r="N147" s="1">
         <v>9</v>
       </c>
-      <c r="N147" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O147" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10515,18 +10654,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K148" s="15">
+      <c r="K148" s="3"/>
+      <c r="L148" s="15">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="M148" s="1">
+      <c r="N148" s="1">
         <v>9</v>
       </c>
-      <c r="N148" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O148" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10555,18 +10695,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K149" s="15">
+      <c r="K149" s="3"/>
+      <c r="L149" s="15">
         <f t="shared" si="12"/>
         <v>33.119999999999997</v>
       </c>
-      <c r="M149" s="1">
+      <c r="N149" s="1">
         <v>9</v>
       </c>
-      <c r="N149" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O149" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10594,18 +10735,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K150" s="15">
+      <c r="K150" s="3"/>
+      <c r="L150" s="15">
         <f t="shared" si="12"/>
         <v>7.1999999999999993</v>
       </c>
-      <c r="M150" s="1">
+      <c r="N150" s="1">
         <v>9</v>
       </c>
-      <c r="N150" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O150" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10633,14 +10775,15 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="K151" s="15">
+      <c r="K151" s="3"/>
+      <c r="L151" s="15">
         <f>D151*(1/(F151*1000/(60*60)))</f>
         <v>6.3</v>
       </c>
-      <c r="M151" s="1" t="s">
+      <c r="N151" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N151" s="1" t="s">
+      <c r="O151" s="1" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
red line logic written
</commit_message>
<xml_diff>
--- a/TrackModelV2/track.xlsx
+++ b/TrackModelV2/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himes\ECE1140\ECE1140\TrackModelV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF420D2-8C89-4616-9346-65FA4AD0876F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60952709-7F86-4109-83CC-BCA7BC33B304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="255" windowWidth="27780" windowHeight="14625" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="630" windowWidth="27780" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="107">
   <si>
     <t>Block Number</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>TC</t>
-  </si>
-  <si>
-    <t>0,1</t>
   </si>
   <si>
     <t>TC num</t>
@@ -1743,9 +1740,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1794,7 @@
         <v>35</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>69</v>
@@ -1831,8 +1828,8 @@
         <v>0.25</v>
       </c>
       <c r="K2" s="3"/>
-      <c r="L2" s="1" t="s">
-        <v>70</v>
+      <c r="L2" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1865,7 +1862,7 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1896,8 +1893,8 @@
         <f t="shared" ref="J4:J67" si="2">I4+J3</f>
         <v>1.5</v>
       </c>
-      <c r="L4" s="9">
-        <v>0</v>
+      <c r="L4" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1929,7 +1926,7 @@
         <v>2.5</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1961,7 +1958,7 @@
         <v>3.25</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1993,7 +1990,7 @@
         <v>3.75</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2017,7 +2014,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>67</v>
@@ -2031,7 +2028,7 @@
         <v>4.125</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2063,7 +2060,7 @@
         <v>4.125</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2086,7 +2083,9 @@
       <c r="F10" s="3">
         <v>40</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="G10" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2095,8 +2094,8 @@
         <f t="shared" si="2"/>
         <v>4.125</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>70</v>
+      <c r="L10" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2119,9 +2118,6 @@
       <c r="F11" s="3">
         <v>40</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="I11" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2131,7 +2127,7 @@
         <v>4.125</v>
       </c>
       <c r="L11" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2163,7 +2159,7 @@
         <v>3.75</v>
       </c>
       <c r="L12" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2195,7 +2191,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2227,7 +2223,7 @@
         <v>1.6</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2259,7 +2255,7 @@
         <v>0.85000000000000009</v>
       </c>
       <c r="L15" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2291,7 +2287,7 @@
         <v>0.25000000000000011</v>
       </c>
       <c r="L16" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2315,7 +2311,7 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>67</v>
@@ -2329,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2361,7 +2357,7 @@
         <v>-1</v>
       </c>
       <c r="L18" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2394,7 +2390,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L19" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2426,7 +2422,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L20" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2458,7 +2454,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L21" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2496,7 +2492,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L22" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2528,7 +2524,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L23" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2560,7 +2556,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L24" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2595,7 +2591,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L25" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2633,7 +2629,7 @@
         <v>-1.2410000000000001</v>
       </c>
       <c r="L26" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2667,6 +2663,9 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
+      <c r="L27" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
@@ -2689,7 +2688,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -2698,6 +2697,9 @@
       <c r="J28" s="12">
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
+      </c>
+      <c r="L28" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2731,6 +2733,9 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
+      <c r="L29" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
@@ -2763,6 +2768,9 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
+      <c r="L30" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
@@ -2795,6 +2803,9 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
+      <c r="L31" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
@@ -2827,8 +2838,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2859,8 +2873,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2881,7 +2898,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I34" s="12">
         <f t="shared" si="0"/>
@@ -2894,8 +2911,11 @@
       <c r="K34" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2926,8 +2946,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2961,8 +2984,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2993,8 +3019,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -3025,8 +3054,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3047,7 +3079,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -3057,8 +3089,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3089,8 +3124,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3121,8 +3159,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3153,8 +3194,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3185,8 +3229,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3217,8 +3264,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3239,7 +3289,7 @@
         <v>70</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I45" s="12">
         <f t="shared" si="0"/>
@@ -3252,8 +3302,11 @@
       <c r="K45" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3287,8 +3340,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3319,8 +3375,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3351,8 +3410,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L48" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3386,8 +3448,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L49" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3415,8 +3480,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L50" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3444,8 +3512,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L51" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3473,8 +3544,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L52" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3495,7 +3569,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -3505,8 +3579,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L53" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3534,8 +3611,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L54" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3563,8 +3643,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L55" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3592,8 +3675,11 @@
         <f t="shared" si="2"/>
         <v>-0.8660000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L56" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3621,8 +3707,11 @@
         <f t="shared" si="2"/>
         <v>-0.4910000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L57" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3650,8 +3739,11 @@
         <f t="shared" si="2"/>
         <v>-0.1160000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L58" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3679,8 +3771,11 @@
         <f t="shared" si="2"/>
         <v>0.6339999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L59" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3708,8 +3803,11 @@
         <f t="shared" si="2"/>
         <v>1.0089999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L60" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3743,8 +3841,11 @@
         <f t="shared" si="2"/>
         <v>1.0089999999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L61" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3772,8 +3873,11 @@
         <f t="shared" si="2"/>
         <v>0.6339999999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L62" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3801,8 +3905,11 @@
         <f t="shared" si="2"/>
         <v>-0.1160000000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L63" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3830,8 +3937,11 @@
         <f t="shared" si="2"/>
         <v>-0.8660000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L64" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3859,8 +3969,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L65" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3888,8 +4001,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L66" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3917,8 +4033,11 @@
         <f t="shared" si="2"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L67" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3949,8 +4068,11 @@
         <f t="shared" ref="J68:J77" si="4">I68+J67</f>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L68" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3981,8 +4103,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L69" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4013,8 +4138,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L70" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A77" si="5">A70</f>
         <v>Red</v>
@@ -4045,8 +4173,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L71" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4077,8 +4208,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L72" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4109,8 +4243,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L73" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4141,8 +4278,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L74" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4173,8 +4313,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L75" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4205,8 +4348,11 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L76" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4237,14 +4383,17 @@
         <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L77" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C78" s="5"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C80" s="5"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
@@ -4479,7 +4628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K1" sqref="K1:K151"/>
     </sheetView>
@@ -4535,10 +4684,10 @@
         <v>61</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4574,10 +4723,10 @@
         <v>8</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -4623,7 +4772,7 @@
         <v>14</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -4664,7 +4813,7 @@
         <v>14</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4704,7 +4853,7 @@
         <v>14</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -4744,7 +4893,7 @@
         <v>14</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -4784,7 +4933,7 @@
         <v>14</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4825,7 +4974,7 @@
         <v>14</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -4865,7 +5014,7 @@
         <v>14</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4911,7 +5060,7 @@
         <v>14</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -4951,7 +5100,7 @@
         <v>14</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4991,7 +5140,7 @@
         <v>14</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -5028,10 +5177,10 @@
         <v>8</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -5055,7 +5204,7 @@
         <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
@@ -5071,10 +5220,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -5111,10 +5260,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -5151,10 +5300,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -5178,7 +5327,7 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>67</v>
@@ -5197,10 +5346,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -5237,10 +5386,10 @@
         <v>9</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -5277,10 +5426,10 @@
         <v>9</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -5320,10 +5469,10 @@
         <v>9</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -5360,10 +5509,10 @@
         <v>9</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -5400,10 +5549,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -5446,10 +5595,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -5486,10 +5635,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -5526,10 +5675,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -5566,10 +5715,10 @@
         <v>10.285714285714286</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -5606,10 +5755,10 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -5646,10 +5795,10 @@
         <v>6</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -5686,10 +5835,10 @@
         <v>6</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -5713,7 +5862,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="1"/>
@@ -5729,10 +5878,10 @@
         <v>6</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -5769,10 +5918,10 @@
         <v>6</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -5818,7 +5967,7 @@
         <v>11</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -5858,7 +6007,7 @@
         <v>11</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -5898,7 +6047,7 @@
         <v>11</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -5938,7 +6087,7 @@
         <v>11</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -5978,7 +6127,7 @@
         <v>11</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -6018,10 +6167,10 @@
         <v>6</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -6064,7 +6213,7 @@
         <v>10</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -6107,7 +6256,7 @@
         <v>10</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -6153,7 +6302,7 @@
         <v>10</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -6196,7 +6345,7 @@
         <v>10</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -6239,7 +6388,7 @@
         <v>10</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -6282,7 +6431,7 @@
         <v>10</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -6325,7 +6474,7 @@
         <v>10</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -6368,7 +6517,7 @@
         <v>10</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -6411,7 +6560,7 @@
         <v>10</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -6454,7 +6603,7 @@
         <v>10</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -6497,7 +6646,7 @@
         <v>10</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -6543,7 +6692,7 @@
         <v>10</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -6586,7 +6735,7 @@
         <v>10</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -6629,7 +6778,7 @@
         <v>10</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -6672,7 +6821,7 @@
         <v>10</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -6715,7 +6864,7 @@
         <v>10</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -6758,7 +6907,7 @@
         <v>10</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -6801,7 +6950,7 @@
         <v>10</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -6844,7 +6993,7 @@
         <v>10</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -6887,7 +7036,7 @@
         <v>10</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
@@ -6911,7 +7060,7 @@
         <v>30</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>68</v>
@@ -6933,7 +7082,7 @@
         <v>10</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -6971,10 +7120,10 @@
         <v>6</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -7014,7 +7163,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -7054,7 +7203,7 @@
         <v>0</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -7094,7 +7243,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -7132,10 +7281,10 @@
         <v>6</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -7159,7 +7308,7 @@
         <v>70</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I64" s="3">
         <f t="shared" si="1"/>
@@ -7178,7 +7327,7 @@
         <v>1</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -7218,7 +7367,7 @@
         <v>1</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -7264,7 +7413,7 @@
         <v>1</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -7304,7 +7453,7 @@
         <v>1</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
@@ -7344,7 +7493,7 @@
         <v>1</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -7381,10 +7530,10 @@
         <v>9</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -7424,7 +7573,7 @@
         <v>2</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -7464,7 +7613,7 @@
         <v>2</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -7504,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -7544,7 +7693,7 @@
         <v>2</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -7590,7 +7739,7 @@
         <v>2</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -7630,7 +7779,7 @@
         <v>2</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -7670,7 +7819,7 @@
         <v>2</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -7707,10 +7856,10 @@
         <v>9</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -7734,7 +7883,7 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>67</v>
@@ -7753,10 +7902,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -7793,10 +7942,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -7833,10 +7982,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -7873,10 +8022,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
@@ -7913,10 +8062,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -7953,10 +8102,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
@@ -7993,10 +8142,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
@@ -8033,10 +8182,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
@@ -8060,7 +8209,7 @@
         <v>70</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I86" s="3">
         <f t="shared" si="8"/>
@@ -8076,10 +8225,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -8116,10 +8265,10 @@
         <v>14.399999999999999</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -8159,7 +8308,7 @@
         <v>5</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -8205,7 +8354,7 @@
         <v>5</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
@@ -8245,7 +8394,7 @@
         <v>5</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
@@ -8285,7 +8434,7 @@
         <v>5</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -8325,7 +8474,7 @@
         <v>5</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -8365,7 +8514,7 @@
         <v>5</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
@@ -8405,7 +8554,7 @@
         <v>5</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -8445,7 +8594,7 @@
         <v>5</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -8485,7 +8634,7 @@
         <v>5</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -8531,7 +8680,7 @@
         <v>5</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -8571,7 +8720,7 @@
         <v>5</v>
       </c>
       <c r="O98" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -8611,7 +8760,7 @@
         <v>5</v>
       </c>
       <c r="O99" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -8651,7 +8800,7 @@
         <v>5</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -8688,10 +8837,10 @@
         <v>10.799999999999999</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -8728,10 +8877,10 @@
         <v>4.8461538461538467</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -8771,7 +8920,7 @@
         <v>6</v>
       </c>
       <c r="O103" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -8811,7 +8960,7 @@
         <v>6</v>
       </c>
       <c r="O104" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -8851,7 +9000,7 @@
         <v>6</v>
       </c>
       <c r="O105" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -8898,7 +9047,7 @@
         <v>6</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -8938,7 +9087,7 @@
         <v>6</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -8978,7 +9127,7 @@
         <v>6</v>
       </c>
       <c r="O108" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -9018,7 +9167,7 @@
         <v>6</v>
       </c>
       <c r="O109" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -9058,7 +9207,7 @@
         <v>6</v>
       </c>
       <c r="O110" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -9095,10 +9244,10 @@
         <v>12</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O111" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -9138,7 +9287,7 @@
         <v>7</v>
       </c>
       <c r="O112" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -9178,7 +9327,7 @@
         <v>7</v>
       </c>
       <c r="O113" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -9218,7 +9367,7 @@
         <v>7</v>
       </c>
       <c r="O114" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -9266,7 +9415,7 @@
         <v>7</v>
       </c>
       <c r="O115" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -9306,7 +9455,7 @@
         <v>7</v>
       </c>
       <c r="O116" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -9346,7 +9495,7 @@
         <v>7</v>
       </c>
       <c r="O117" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -9386,7 +9535,7 @@
         <v>7</v>
       </c>
       <c r="O118" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -9426,7 +9575,7 @@
         <v>7</v>
       </c>
       <c r="O119" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
@@ -9466,7 +9615,7 @@
         <v>7</v>
       </c>
       <c r="O120" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -9506,7 +9655,7 @@
         <v>7</v>
       </c>
       <c r="O121" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
@@ -9546,7 +9695,7 @@
         <v>7</v>
       </c>
       <c r="O122" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
@@ -9586,10 +9735,10 @@
         <v>9</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O123" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -9613,7 +9762,7 @@
         <v>20</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>68</v>
@@ -9635,7 +9784,7 @@
         <v>8</v>
       </c>
       <c r="O124" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -9678,7 +9827,7 @@
         <v>8</v>
       </c>
       <c r="O125" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
@@ -9721,7 +9870,7 @@
         <v>8</v>
       </c>
       <c r="O126" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -9764,7 +9913,7 @@
         <v>8</v>
       </c>
       <c r="O127" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
@@ -9807,7 +9956,7 @@
         <v>8</v>
       </c>
       <c r="O128" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
@@ -9850,7 +9999,7 @@
         <v>8</v>
       </c>
       <c r="O129" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
@@ -9893,7 +10042,7 @@
         <v>8</v>
       </c>
       <c r="O130" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
@@ -9936,7 +10085,7 @@
         <v>8</v>
       </c>
       <c r="O131" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
@@ -9979,7 +10128,7 @@
         <v>8</v>
       </c>
       <c r="O132" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="133" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -10026,7 +10175,7 @@
         <v>8</v>
       </c>
       <c r="O133" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
@@ -10069,7 +10218,7 @@
         <v>8</v>
       </c>
       <c r="O134" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
@@ -10112,7 +10261,7 @@
         <v>8</v>
       </c>
       <c r="O135" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
@@ -10155,7 +10304,7 @@
         <v>8</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
@@ -10198,7 +10347,7 @@
         <v>8</v>
       </c>
       <c r="O137" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
@@ -10241,7 +10390,7 @@
         <v>8</v>
       </c>
       <c r="O138" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
@@ -10284,7 +10433,7 @@
         <v>8</v>
       </c>
       <c r="O139" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
@@ -10327,7 +10476,7 @@
         <v>8</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
@@ -10370,7 +10519,7 @@
         <v>8</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -10417,7 +10566,7 @@
         <v>8</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
@@ -10460,7 +10609,7 @@
         <v>8</v>
       </c>
       <c r="O143" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
@@ -10503,7 +10652,7 @@
         <v>8</v>
       </c>
       <c r="O144" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
@@ -10540,10 +10689,10 @@
         <v>9</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
@@ -10583,7 +10732,7 @@
         <v>9</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
@@ -10623,7 +10772,7 @@
         <v>9</v>
       </c>
       <c r="O147" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
@@ -10663,7 +10812,7 @@
         <v>9</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
@@ -10704,7 +10853,7 @@
         <v>9</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
@@ -10744,7 +10893,7 @@
         <v>9</v>
       </c>
       <c r="O150" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
@@ -10781,10 +10930,10 @@
         <v>6.3</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>